<commit_message>
Adição dos parâmetros considerando agoras as 18 curvas
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -685,16 +685,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1013</v>
+        <v>1021</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1090</v>
+        <v>1106</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -718,7 +718,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>747</v>
+        <v>740</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Adicionei uma linha que pode ajudar a implementar o programa para um número n de segmentos
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -2,6 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Patient</t>
   </si>
@@ -66,9 +67,6 @@
   </si>
   <si>
     <t>Aristoteles</t>
-  </si>
-  <si>
-    <t>Valores antigos</t>
   </si>
   <si>
     <t>Electrical Mechanical Coupling = Onset QRS – MVC (Troquei a ordem)</t>
@@ -186,12 +184,12 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
@@ -234,7 +232,6 @@
     <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
     <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -527,28 +524,28 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="F1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
-      <selection activeCell="K4" activeCellId="0" pane="topLeft" sqref="K4"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
+      <selection activeCell="A9" activeCellId="0" pane="topLeft" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="12.2857142857143"/>
-    <col customWidth="1" max="6" min="2" style="1" width="9.852040816326531"/>
-    <col customWidth="1" max="7" min="7" style="1" width="19.8418367346939"/>
-    <col customWidth="1" max="8" min="8" style="1" width="21.0612244897959"/>
-    <col customWidth="1" max="9" min="9" style="1" width="17.280612244898"/>
-    <col customWidth="1" max="10" min="10" style="1" width="16.6020408163265"/>
-    <col customWidth="1" max="11" min="11" style="1" width="17.5510204081633"/>
-    <col customWidth="1" max="12" min="12" style="1" width="24.4336734693878"/>
-    <col customWidth="1" max="13" min="13" style="1" width="13.0918367346939"/>
-    <col customWidth="1" max="14" min="14" style="1" width="22.9489795918367"/>
-    <col customWidth="1" max="15" min="15" style="1" width="17.280612244898"/>
-    <col customWidth="1" max="16" min="16" style="1" width="14.5816326530612"/>
-    <col customWidth="1" max="18" min="17" style="1" width="15.5255102040816"/>
-    <col customWidth="1" max="1025" min="19" style="1" width="9.852040816326531"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.29"/>
+    <col customWidth="1" max="6" min="2" style="1" width="9.85"/>
+    <col customWidth="1" max="7" min="7" style="1" width="19.84"/>
+    <col customWidth="1" max="8" min="8" style="1" width="21.06"/>
+    <col customWidth="1" max="9" min="9" style="1" width="17.28"/>
+    <col customWidth="1" max="10" min="10" style="1" width="16.6"/>
+    <col customWidth="1" max="11" min="11" style="1" width="17.55"/>
+    <col customWidth="1" max="12" min="12" style="1" width="24.43"/>
+    <col customWidth="1" max="13" min="13" style="1" width="13.09"/>
+    <col customWidth="1" max="14" min="14" style="1" width="22.95"/>
+    <col customWidth="1" max="15" min="15" style="1" width="17.28"/>
+    <col customWidth="1" max="16" min="16" style="1" width="14.58"/>
+    <col customWidth="1" max="18" min="17" style="1" width="15.53"/>
+    <col customWidth="1" max="1025" min="19" style="1" width="9.85"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="10" spans="1:26">
@@ -685,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -718,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>740</v>
+        <v>751</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>
@@ -733,550 +730,20 @@
       <c r="Y4" s="2" t="n"/>
       <c r="Z4" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5" s="10" spans="1:26">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>1144</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>1026</v>
-      </c>
-      <c r="J5" s="6" t="n">
-        <v>1104</v>
-      </c>
-      <c r="K5" s="7" t="n"/>
-      <c r="L5" s="3">
-        <f>G5-D5</f>
-        <v/>
-      </c>
-      <c r="M5" s="3">
-        <f>E5-D5</f>
-        <v/>
-      </c>
-      <c r="N5" s="3">
-        <f>F5-E5</f>
-        <v/>
-      </c>
-      <c r="O5" s="3">
-        <f>C5-F5</f>
-        <v/>
-      </c>
-      <c r="P5" s="3">
-        <f>I5-C5</f>
-        <v/>
-      </c>
-      <c r="Q5" s="7" t="n">
-        <v>740</v>
-      </c>
-      <c r="R5" s="3">
-        <f>J5-I5</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="6" s="10" spans="1:26">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>79</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>1062</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>950</v>
-      </c>
-      <c r="J6" s="6" t="n">
-        <v>1021</v>
-      </c>
-      <c r="K6" s="7" t="n"/>
-      <c r="L6" s="3">
-        <f>G6-D6</f>
-        <v/>
-      </c>
-      <c r="M6" s="3">
-        <f>E6-D6</f>
-        <v/>
-      </c>
-      <c r="N6" s="3">
-        <f>F6-E6</f>
-        <v/>
-      </c>
-      <c r="O6" s="3">
-        <f>C6-F6</f>
-        <v/>
-      </c>
-      <c r="P6" s="3">
-        <f>I6-C6</f>
-        <v/>
-      </c>
-      <c r="Q6" s="7" t="n"/>
-      <c r="R6" s="3">
-        <f>J6-I6</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="10" spans="1:26">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I7" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K7" s="7" t="n"/>
-      <c r="L7" s="3">
-        <f>G7-D7</f>
-        <v/>
-      </c>
-      <c r="M7" s="3">
-        <f>E7-D7</f>
-        <v/>
-      </c>
-      <c r="N7" s="3">
-        <f>F7-E7</f>
-        <v/>
-      </c>
-      <c r="O7" s="3">
-        <f>C7-F7</f>
-        <v/>
-      </c>
-      <c r="P7" s="3">
-        <f>I7-C7</f>
-        <v/>
-      </c>
-      <c r="Q7" s="7" t="n"/>
-      <c r="R7" s="3">
-        <f>J7-I7</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="8" s="10" spans="1:26">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H8" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I8" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J8" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K8" s="7" t="n"/>
-      <c r="L8" s="3">
-        <f>G8-D8</f>
-        <v/>
-      </c>
-      <c r="M8" s="3">
-        <f>E8-D8</f>
-        <v/>
-      </c>
-      <c r="N8" s="3">
-        <f>F8-E8</f>
-        <v/>
-      </c>
-      <c r="O8" s="3">
-        <f>C8-F8</f>
-        <v/>
-      </c>
-      <c r="P8" s="3">
-        <f>I8-C8</f>
-        <v/>
-      </c>
-      <c r="Q8" s="7" t="n"/>
-      <c r="R8" s="3">
-        <f>J8-I8</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="10" spans="1:26">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H9" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I9" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J9" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K9" s="7" t="n"/>
-      <c r="L9" s="3">
-        <f>G9-D9</f>
-        <v/>
-      </c>
-      <c r="M9" s="3">
-        <f>E9-D9</f>
-        <v/>
-      </c>
-      <c r="N9" s="3">
-        <f>F9-E9</f>
-        <v/>
-      </c>
-      <c r="O9" s="3">
-        <f>C9-F9</f>
-        <v/>
-      </c>
-      <c r="P9" s="3">
-        <f>I9-C9</f>
-        <v/>
-      </c>
-      <c r="Q9" s="7" t="n"/>
-      <c r="R9" s="3">
-        <f>J9-I9</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="10" s="10" spans="1:26">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G10" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H10" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I10" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K10" s="7" t="n"/>
-      <c r="L10" s="3">
-        <f>G10-D10</f>
-        <v/>
-      </c>
-      <c r="M10" s="3">
-        <f>E10-D10</f>
-        <v/>
-      </c>
-      <c r="N10" s="3">
-        <f>F10-E10</f>
-        <v/>
-      </c>
-      <c r="O10" s="3">
-        <f>C10-F10</f>
-        <v/>
-      </c>
-      <c r="P10" s="3">
-        <f>I10-C10</f>
-        <v/>
-      </c>
-      <c r="Q10" s="7" t="n"/>
-      <c r="R10" s="3">
-        <f>J10-I10</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="11" s="10" spans="1:26">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F11" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G11" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H11" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I11" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J11" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K11" s="7" t="n"/>
-      <c r="L11" s="3">
-        <f>G11-D11</f>
-        <v/>
-      </c>
-      <c r="M11" s="3">
-        <f>E11-D11</f>
-        <v/>
-      </c>
-      <c r="N11" s="3">
-        <f>F11-E11</f>
-        <v/>
-      </c>
-      <c r="O11" s="3">
-        <f>C11-F11</f>
-        <v/>
-      </c>
-      <c r="P11" s="3">
-        <f>I11-C11</f>
-        <v/>
-      </c>
-      <c r="Q11" s="7" t="n"/>
-      <c r="R11" s="3">
-        <f>J11-I11</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="12" s="10" spans="1:26">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E12" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F12" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H12" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I12" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J12" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K12" s="7" t="n"/>
-      <c r="L12" s="3">
-        <f>G12-D12</f>
-        <v/>
-      </c>
-      <c r="M12" s="3">
-        <f>E12-D12</f>
-        <v/>
-      </c>
-      <c r="N12" s="3">
-        <f>F12-E12</f>
-        <v/>
-      </c>
-      <c r="O12" s="3">
-        <f>C12-F12</f>
-        <v/>
-      </c>
-      <c r="P12" s="3">
-        <f>I12-C12</f>
-        <v/>
-      </c>
-      <c r="Q12" s="7" t="n"/>
-      <c r="R12" s="3">
-        <f>J12-I12</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="13" s="10" spans="1:26">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="n"/>
-      <c r="C13" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G13" s="3" t="n">
-        <v>143</v>
-      </c>
-      <c r="H13" s="3" t="n">
-        <v>205</v>
-      </c>
-      <c r="I13" s="3" t="n">
-        <v>922</v>
-      </c>
-      <c r="J13" s="6" t="n">
-        <v>1102</v>
-      </c>
-      <c r="K13" s="7" t="n"/>
-      <c r="L13" s="3">
-        <f>G13-D13</f>
-        <v/>
-      </c>
-      <c r="M13" s="3">
-        <f>E13-D13</f>
-        <v/>
-      </c>
-      <c r="N13" s="3">
-        <f>F13-E13</f>
-        <v/>
-      </c>
-      <c r="O13" s="3">
-        <f>C13-F13</f>
-        <v/>
-      </c>
-      <c r="P13" s="3">
-        <f>I13-C13</f>
-        <v/>
-      </c>
-      <c r="Q13" s="7" t="n"/>
-      <c r="R13" s="3">
-        <f>J13-I13</f>
-        <v/>
-      </c>
-    </row>
+    <row customHeight="1" ht="15" r="5" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="6" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="7" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="8" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="9" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="10" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="11" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="12" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="13" s="10" spans="1:26"/>
     <row customHeight="1" ht="19.7" r="16" s="10" spans="1:26"/>
     <row customHeight="1" ht="15" r="17" s="10" spans="1:26"/>
     <row customHeight="1" ht="15" r="18" s="10" spans="1:26"/>
-    <row customHeight="1" ht="15" r="24" s="10" spans="1:26">
-      <c r="A24" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="25" s="10" spans="1:26">
-      <c r="A25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="3" t="n"/>
-      <c r="C25" s="3" t="n">
-        <v>453</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="E25" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="F25" s="3" t="n">
-        <v>382</v>
-      </c>
-      <c r="G25" s="3" t="n">
-        <v>141</v>
-      </c>
-      <c r="H25" s="3" t="n">
-        <v>203</v>
-      </c>
-      <c r="I25" s="3" t="n">
-        <v>904</v>
-      </c>
-      <c r="J25" s="6" t="n">
-        <v>1090</v>
-      </c>
-    </row>
+    <row customHeight="1" ht="15" r="24" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="25" s="10" spans="1:26"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="1" verticalCentered="1"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
@@ -1300,48 +767,48 @@
   </sheetPr>
   <dimension ref="B4:B17"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A2" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A2" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E17" activeCellId="0" pane="topLeft" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="9" width="10.1224489795918"/>
+    <col customWidth="1" max="1025" min="1" style="9" width="10.12"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="4" s="10" spans="1:2">
       <c r="B4" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="6" s="10" spans="1:2">
       <c r="B6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="9" s="10" spans="1:2">
       <c r="B9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="11" s="10" spans="1:2">
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="13" s="10" spans="1:2">
       <c r="B13" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="15" s="10" spans="1:2">
       <c r="B15" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="17" s="10" spans="1:2">
       <c r="B17" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculo dos parâmetros para 18 segmentos de strain, arquivo a ser enviado para testes
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -682,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1145</v>
+        <v>1086</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1021</v>
+        <v>1004</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1110</v>
+        <v>1050</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Versao apresentada no Dante
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -682,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>801</v>
+        <v>809</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Alteracoes visuais: Linha e impressoes em DR
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -682,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1101</v>
+        <v>1106</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Parametros para menos de 18 curvas
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -685,13 +685,13 @@
         <v>98</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1031</v>
+        <v>1023</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1106</v>
+        <v>1099</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>723</v>
+        <v>705</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Alteração na impressão DR
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -682,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1013</v>
+        <v>1001</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Medida do desvio padrão - Diastolic Index
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -682,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1135</v>
+        <v>1140</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1001</v>
+        <v>1022</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">

</xml_diff>

<commit_message>
Preparação para a implementação do bullseye
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -688,10 +688,10 @@
         <v>1134</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1031</v>
+        <v>1021</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>702</v>
+        <v>742</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Correção do bullseye 18 seg
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -682,16 +682,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1137</v>
+        <v>1142</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1012</v>
+        <v>1025</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>753</v>
+        <v>713</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Alteração da linha sheet=wb ...
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -94,9 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="General" numFmtId="164"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="9">
     <font>
       <name val="Arial"/>
@@ -191,38 +189,65 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="20">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -532,203 +557,203 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="12.29"/>
-    <col customWidth="1" max="6" min="2" style="1" width="9.85"/>
-    <col customWidth="1" max="7" min="7" style="1" width="19.84"/>
-    <col customWidth="1" max="8" min="8" style="1" width="21.06"/>
-    <col customWidth="1" max="9" min="9" style="1" width="17.28"/>
-    <col customWidth="1" max="10" min="10" style="1" width="16.6"/>
-    <col customWidth="1" max="11" min="11" style="1" width="17.55"/>
-    <col customWidth="1" max="12" min="12" style="1" width="24.43"/>
-    <col customWidth="1" max="13" min="13" style="1" width="13.09"/>
-    <col customWidth="1" max="14" min="14" style="1" width="22.95"/>
-    <col customWidth="1" max="15" min="15" style="1" width="17.28"/>
-    <col customWidth="1" max="16" min="16" style="1" width="14.58"/>
-    <col customWidth="1" max="18" min="17" style="1" width="15.53"/>
-    <col customWidth="1" max="1025" min="19" style="1" width="9.85"/>
+    <col customWidth="1" max="1" min="1" style="11" width="12.29"/>
+    <col customWidth="1" max="6" min="2" style="11" width="9.85"/>
+    <col customWidth="1" max="7" min="7" style="11" width="19.84"/>
+    <col customWidth="1" max="8" min="8" style="11" width="21.06"/>
+    <col customWidth="1" max="9" min="9" style="11" width="17.28"/>
+    <col customWidth="1" max="10" min="10" style="11" width="16.6"/>
+    <col customWidth="1" max="11" min="11" style="11" width="17.55"/>
+    <col customWidth="1" max="12" min="12" style="11" width="24.43"/>
+    <col customWidth="1" max="13" min="13" style="11" width="13.09"/>
+    <col customWidth="1" max="14" min="14" style="11" width="22.95"/>
+    <col customWidth="1" max="15" min="15" style="11" width="17.28"/>
+    <col customWidth="1" max="16" min="16" style="11" width="14.58"/>
+    <col customWidth="1" max="18" min="17" style="11" width="15.53"/>
+    <col customWidth="1" max="1025" min="19" style="11" width="9.85"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="10" spans="1:26">
-      <c r="A1" s="2" t="n"/>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="2" t="n"/>
-      <c r="Q1" s="2" t="n"/>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="2" t="n"/>
-      <c r="T1" s="2" t="n"/>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="2" t="n"/>
-      <c r="W1" s="2" t="n"/>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="2" t="n"/>
-      <c r="Z1" s="2" t="n"/>
+      <c r="A1" s="12" t="n"/>
+      <c r="B1" s="12" t="n"/>
+      <c r="C1" s="12" t="n"/>
+      <c r="D1" s="12" t="n"/>
+      <c r="E1" s="12" t="n"/>
+      <c r="F1" s="12" t="n"/>
+      <c r="G1" s="12" t="n"/>
+      <c r="H1" s="12" t="n"/>
+      <c r="I1" s="12" t="n"/>
+      <c r="J1" s="12" t="n"/>
+      <c r="K1" s="12" t="n"/>
+      <c r="L1" s="12" t="n"/>
+      <c r="M1" s="12" t="n"/>
+      <c r="N1" s="12" t="n"/>
+      <c r="O1" s="12" t="n"/>
+      <c r="P1" s="12" t="n"/>
+      <c r="Q1" s="12" t="n"/>
+      <c r="R1" s="12" t="n"/>
+      <c r="S1" s="12" t="n"/>
+      <c r="T1" s="12" t="n"/>
+      <c r="U1" s="12" t="n"/>
+      <c r="V1" s="12" t="n"/>
+      <c r="W1" s="12" t="n"/>
+      <c r="X1" s="12" t="n"/>
+      <c r="Y1" s="12" t="n"/>
+      <c r="Z1" s="12" t="n"/>
     </row>
     <row customHeight="1" ht="19.7" r="2" s="10" spans="1:26">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="n"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="13" t="n"/>
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="n"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="14" t="n"/>
+      <c r="L2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="2" t="n"/>
-      <c r="T2" s="2" t="n"/>
-      <c r="U2" s="2" t="n"/>
-      <c r="V2" s="2" t="n"/>
-      <c r="W2" s="2" t="n"/>
-      <c r="X2" s="2" t="n"/>
-      <c r="Y2" s="2" t="n"/>
-      <c r="Z2" s="2" t="n"/>
+      <c r="S2" s="12" t="n"/>
+      <c r="T2" s="12" t="n"/>
+      <c r="U2" s="12" t="n"/>
+      <c r="V2" s="12" t="n"/>
+      <c r="W2" s="12" t="n"/>
+      <c r="X2" s="12" t="n"/>
+      <c r="Y2" s="12" t="n"/>
+      <c r="Z2" s="12" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="3" s="10" spans="1:26">
-      <c r="A3" s="3" t="n"/>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="6" t="n"/>
-      <c r="L3" s="3" t="n"/>
-      <c r="M3" s="3" t="n"/>
-      <c r="N3" s="3" t="n"/>
-      <c r="O3" s="3" t="n"/>
-      <c r="P3" s="3" t="n"/>
-      <c r="Q3" s="3" t="n"/>
-      <c r="R3" s="3" t="n"/>
-      <c r="S3" s="2" t="n"/>
-      <c r="T3" s="2" t="n"/>
-      <c r="U3" s="2" t="n"/>
-      <c r="V3" s="2" t="n"/>
-      <c r="W3" s="2" t="n"/>
-      <c r="X3" s="2" t="n"/>
-      <c r="Y3" s="2" t="n"/>
-      <c r="Z3" s="2" t="n"/>
+      <c r="A3" s="13" t="n"/>
+      <c r="B3" s="13" t="n"/>
+      <c r="C3" s="13" t="n"/>
+      <c r="D3" s="13" t="n"/>
+      <c r="E3" s="13" t="n"/>
+      <c r="F3" s="13" t="n"/>
+      <c r="G3" s="13" t="n"/>
+      <c r="H3" s="13" t="n"/>
+      <c r="I3" s="13" t="n"/>
+      <c r="J3" s="16" t="n"/>
+      <c r="K3" s="16" t="n"/>
+      <c r="L3" s="13" t="n"/>
+      <c r="M3" s="13" t="n"/>
+      <c r="N3" s="13" t="n"/>
+      <c r="O3" s="13" t="n"/>
+      <c r="P3" s="13" t="n"/>
+      <c r="Q3" s="13" t="n"/>
+      <c r="R3" s="13" t="n"/>
+      <c r="S3" s="12" t="n"/>
+      <c r="T3" s="12" t="n"/>
+      <c r="U3" s="12" t="n"/>
+      <c r="V3" s="12" t="n"/>
+      <c r="W3" s="12" t="n"/>
+      <c r="X3" s="12" t="n"/>
+      <c r="Y3" s="12" t="n"/>
+      <c r="Z3" s="12" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="4" s="10" spans="1:26">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n">
+      <c r="B4" s="13" t="n"/>
+      <c r="C4" s="13" t="n">
         <v>453</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="13" t="n">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="13" t="n">
         <v>72</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="13" t="n">
         <v>382</v>
       </c>
-      <c r="G4" s="3" t="n">
-        <v>103</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>1136</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>1013</v>
-      </c>
-      <c r="J4" s="6" t="n">
-        <v>1101</v>
-      </c>
-      <c r="K4" s="7" t="n"/>
-      <c r="L4" s="3">
+      <c r="G4" s="13" t="n">
+        <v>107</v>
+      </c>
+      <c r="H4" s="13" t="n">
+        <v>1143</v>
+      </c>
+      <c r="I4" s="13" t="n">
+        <v>1011</v>
+      </c>
+      <c r="J4" s="16" t="n">
+        <v>1103</v>
+      </c>
+      <c r="K4" s="17" t="n"/>
+      <c r="L4" s="13">
         <f>G4-D4</f>
         <v/>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="13">
         <f>E4-D4</f>
         <v/>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="13">
         <f>F4-E4</f>
         <v/>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="13">
         <f>C4-F4</f>
         <v/>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="13">
         <f>I4-C4</f>
         <v/>
       </c>
-      <c r="Q4" s="3" t="n">
-        <v>692</v>
-      </c>
-      <c r="R4" s="3">
+      <c r="Q4" s="13" t="n">
+        <v>721</v>
+      </c>
+      <c r="R4" s="13">
         <f>J4-I4</f>
         <v/>
       </c>
-      <c r="S4" s="8" t="n"/>
-      <c r="T4" s="8" t="n"/>
-      <c r="U4" s="2" t="n"/>
-      <c r="V4" s="2" t="n"/>
-      <c r="W4" s="2" t="n"/>
-      <c r="X4" s="2" t="n"/>
-      <c r="Y4" s="2" t="n"/>
-      <c r="Z4" s="2" t="n"/>
+      <c r="S4" s="18" t="n"/>
+      <c r="T4" s="18" t="n"/>
+      <c r="U4" s="12" t="n"/>
+      <c r="V4" s="12" t="n"/>
+      <c r="W4" s="12" t="n"/>
+      <c r="X4" s="12" t="n"/>
+      <c r="Y4" s="12" t="n"/>
+      <c r="Z4" s="12" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="5" s="10" spans="1:26"/>
     <row customHeight="1" ht="15" r="6" s="10" spans="1:26"/>
@@ -773,41 +798,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="9" width="10.12"/>
+    <col customWidth="1" max="1025" min="1" style="19" width="10.12"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="4" s="10" spans="1:2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="6" s="10" spans="1:2">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="9" s="10" spans="1:2">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="11" s="10" spans="1:2">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="13" s="10" spans="1:2">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="15" s="10" spans="1:2">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="17" s="10" spans="1:2">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="19" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit antes de trocar de branch
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -707,16 +707,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="13" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H4" s="13" t="n">
-        <v>1140</v>
+        <v>1145</v>
       </c>
       <c r="I4" s="13" t="n">
-        <v>1030</v>
+        <v>1012</v>
       </c>
       <c r="J4" s="16" t="n">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="K4" s="17" t="n"/>
       <c r="L4" s="13">
@@ -740,7 +740,7 @@
         <v/>
       </c>
       <c r="Q4" s="13" t="n">
-        <v>718</v>
+        <v>734</v>
       </c>
       <c r="R4" s="13">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Ocultação dos segmentos globais - Ajustes para arquivos de simulações
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -707,16 +707,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="13" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="H4" s="13" t="n">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="I4" s="13" t="n">
-        <v>1030</v>
+        <v>1011</v>
       </c>
       <c r="J4" s="16" t="n">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="K4" s="17" t="n"/>
       <c r="L4" s="13">
@@ -740,7 +740,7 @@
         <v/>
       </c>
       <c r="Q4" s="13" t="n">
-        <v>718</v>
+        <v>738</v>
       </c>
       <c r="R4" s="13">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Arrumar diastolic index para um número menor que 18 de segmentos.
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -66,7 +66,7 @@
     <t>A</t>
   </si>
   <si>
-    <t>Aristoteles</t>
+    <t>Sim_LBBB</t>
   </si>
   <si>
     <t>Electrical Mechanical Coupling = Onset QRS – MVC (Troquei a ordem)</t>
@@ -94,7 +94,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="General" numFmtId="164"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <name val="Arial"/>
@@ -189,65 +191,38 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="11">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -552,208 +527,208 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="I9" activeCellId="0" pane="topLeft" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="12.29"/>
-    <col customWidth="1" max="6" min="2" style="11" width="9.85"/>
-    <col customWidth="1" max="7" min="7" style="11" width="19.84"/>
-    <col customWidth="1" max="8" min="8" style="11" width="21.06"/>
-    <col customWidth="1" max="9" min="9" style="11" width="17.28"/>
-    <col customWidth="1" max="10" min="10" style="11" width="16.6"/>
-    <col customWidth="1" max="11" min="11" style="11" width="17.55"/>
-    <col customWidth="1" max="12" min="12" style="11" width="24.43"/>
-    <col customWidth="1" max="13" min="13" style="11" width="13.09"/>
-    <col customWidth="1" max="14" min="14" style="11" width="22.95"/>
-    <col customWidth="1" max="15" min="15" style="11" width="17.28"/>
-    <col customWidth="1" max="16" min="16" style="11" width="14.58"/>
-    <col customWidth="1" max="18" min="17" style="11" width="15.53"/>
-    <col customWidth="1" max="1025" min="19" style="11" width="9.85"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.29"/>
+    <col customWidth="1" max="6" min="2" style="1" width="9.85"/>
+    <col customWidth="1" max="7" min="7" style="1" width="19.84"/>
+    <col customWidth="1" max="8" min="8" style="1" width="21.06"/>
+    <col customWidth="1" max="9" min="9" style="1" width="17.28"/>
+    <col customWidth="1" max="10" min="10" style="1" width="16.6"/>
+    <col customWidth="1" max="11" min="11" style="1" width="17.55"/>
+    <col customWidth="1" max="12" min="12" style="1" width="24.42"/>
+    <col customWidth="1" max="13" min="13" style="1" width="13.09"/>
+    <col customWidth="1" max="14" min="14" style="1" width="22.95"/>
+    <col customWidth="1" max="15" min="15" style="1" width="17.28"/>
+    <col customWidth="1" max="16" min="16" style="1" width="14.58"/>
+    <col customWidth="1" max="18" min="17" style="1" width="15.53"/>
+    <col customWidth="1" max="1025" min="19" style="1" width="9.85"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="10" spans="1:26">
-      <c r="A1" s="12" t="n"/>
-      <c r="B1" s="12" t="n"/>
-      <c r="C1" s="12" t="n"/>
-      <c r="D1" s="12" t="n"/>
-      <c r="E1" s="12" t="n"/>
-      <c r="F1" s="12" t="n"/>
-      <c r="G1" s="12" t="n"/>
-      <c r="H1" s="12" t="n"/>
-      <c r="I1" s="12" t="n"/>
-      <c r="J1" s="12" t="n"/>
-      <c r="K1" s="12" t="n"/>
-      <c r="L1" s="12" t="n"/>
-      <c r="M1" s="12" t="n"/>
-      <c r="N1" s="12" t="n"/>
-      <c r="O1" s="12" t="n"/>
-      <c r="P1" s="12" t="n"/>
-      <c r="Q1" s="12" t="n"/>
-      <c r="R1" s="12" t="n"/>
-      <c r="S1" s="12" t="n"/>
-      <c r="T1" s="12" t="n"/>
-      <c r="U1" s="12" t="n"/>
-      <c r="V1" s="12" t="n"/>
-      <c r="W1" s="12" t="n"/>
-      <c r="X1" s="12" t="n"/>
-      <c r="Y1" s="12" t="n"/>
-      <c r="Z1" s="12" t="n"/>
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="19.7" r="2" s="10" spans="1:26">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="n"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="n"/>
-      <c r="L2" s="15" t="s">
+      <c r="K2" s="4" t="n"/>
+      <c r="L2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="P2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="12" t="n"/>
-      <c r="T2" s="12" t="n"/>
-      <c r="U2" s="12" t="n"/>
-      <c r="V2" s="12" t="n"/>
-      <c r="W2" s="12" t="n"/>
-      <c r="X2" s="12" t="n"/>
-      <c r="Y2" s="12" t="n"/>
-      <c r="Z2" s="12" t="n"/>
+      <c r="S2" s="2" t="n"/>
+      <c r="T2" s="2" t="n"/>
+      <c r="U2" s="2" t="n"/>
+      <c r="V2" s="2" t="n"/>
+      <c r="W2" s="2" t="n"/>
+      <c r="X2" s="2" t="n"/>
+      <c r="Y2" s="2" t="n"/>
+      <c r="Z2" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="3" s="10" spans="1:26">
-      <c r="A3" s="13" t="n"/>
-      <c r="B3" s="13" t="n"/>
-      <c r="C3" s="13" t="n"/>
-      <c r="D3" s="13" t="n"/>
-      <c r="E3" s="13" t="n"/>
-      <c r="F3" s="13" t="n"/>
-      <c r="G3" s="13" t="n"/>
-      <c r="H3" s="13" t="n"/>
-      <c r="I3" s="13" t="n"/>
-      <c r="J3" s="16" t="n"/>
-      <c r="K3" s="16" t="n"/>
-      <c r="L3" s="13" t="n"/>
-      <c r="M3" s="13" t="n"/>
-      <c r="N3" s="13" t="n"/>
-      <c r="O3" s="13" t="n"/>
-      <c r="P3" s="13" t="n"/>
-      <c r="Q3" s="13" t="n"/>
-      <c r="R3" s="13" t="n"/>
-      <c r="S3" s="12" t="n"/>
-      <c r="T3" s="12" t="n"/>
-      <c r="U3" s="12" t="n"/>
-      <c r="V3" s="12" t="n"/>
-      <c r="W3" s="12" t="n"/>
-      <c r="X3" s="12" t="n"/>
-      <c r="Y3" s="12" t="n"/>
-      <c r="Z3" s="12" t="n"/>
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="6" t="n"/>
+      <c r="K3" s="6" t="n"/>
+      <c r="L3" s="3" t="n"/>
+      <c r="M3" s="3" t="n"/>
+      <c r="N3" s="3" t="n"/>
+      <c r="O3" s="3" t="n"/>
+      <c r="P3" s="3" t="n"/>
+      <c r="Q3" s="3" t="n"/>
+      <c r="R3" s="3" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
+      <c r="U3" s="2" t="n"/>
+      <c r="V3" s="2" t="n"/>
+      <c r="W3" s="2" t="n"/>
+      <c r="X3" s="2" t="n"/>
+      <c r="Y3" s="2" t="n"/>
+      <c r="Z3" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="4" s="10" spans="1:26">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="13" t="n"/>
-      <c r="C4" s="13" t="n">
-        <v>453</v>
-      </c>
-      <c r="D4" s="13" t="n">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="n">
-        <v>72</v>
-      </c>
-      <c r="F4" s="13" t="n">
-        <v>382</v>
-      </c>
-      <c r="G4" s="13" t="n">
-        <v>100</v>
-      </c>
-      <c r="H4" s="13" t="n">
-        <v>1140</v>
-      </c>
-      <c r="I4" s="13" t="n">
-        <v>1026</v>
-      </c>
-      <c r="J4" s="16" t="n">
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n">
+        <v>714</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>257</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>318</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>640</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>103</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>1145</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>1022</v>
+      </c>
+      <c r="J4" s="6" t="n">
         <v>1107</v>
       </c>
-      <c r="K4" s="17" t="n"/>
-      <c r="L4" s="13">
+      <c r="K4" s="7" t="n"/>
+      <c r="L4" s="3">
         <f>G4-D4</f>
         <v/>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="3">
         <f>E4-D4</f>
         <v/>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="3">
         <f>F4-E4</f>
         <v/>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="3">
         <f>C4-F4</f>
         <v/>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="3">
         <f>I4-C4</f>
         <v/>
       </c>
-      <c r="Q4" s="13" t="n">
-        <v>735</v>
-      </c>
-      <c r="R4" s="13">
+      <c r="Q4" s="3" t="n">
+        <v>709</v>
+      </c>
+      <c r="R4" s="3">
         <f>J4-I4</f>
         <v/>
       </c>
-      <c r="S4" s="18" t="n"/>
-      <c r="T4" s="18" t="n"/>
-      <c r="U4" s="12" t="n"/>
-      <c r="V4" s="12" t="n"/>
-      <c r="W4" s="12" t="n"/>
-      <c r="X4" s="12" t="n"/>
-      <c r="Y4" s="12" t="n"/>
-      <c r="Z4" s="12" t="n"/>
+      <c r="S4" s="8" t="n"/>
+      <c r="T4" s="8" t="n"/>
+      <c r="U4" s="2" t="n"/>
+      <c r="V4" s="2" t="n"/>
+      <c r="W4" s="2" t="n"/>
+      <c r="X4" s="2" t="n"/>
+      <c r="Y4" s="2" t="n"/>
+      <c r="Z4" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="5" s="10" spans="1:26"/>
     <row customHeight="1" ht="15" r="6" s="10" spans="1:26"/>
@@ -798,41 +773,41 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="19" width="10.12"/>
+    <col customWidth="1" max="1025" min="1" style="9" width="10.12"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="4" s="10" spans="1:2">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="6" s="10" spans="1:2">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="9" s="10" spans="1:2">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="11" s="10" spans="1:2">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="13" s="10" spans="1:2">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="15" s="10" spans="1:2">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="17" s="10" spans="1:2">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="9" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Diastolic Index funcional, falta o bull's eye para simulacoes
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -682,16 +682,16 @@
         <v>640</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1022</v>
+        <v>1010</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>1107</v>
+        <v>1102</v>
       </c>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="3">
@@ -715,7 +715,7 @@
         <v/>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>655</v>
+        <v>722</v>
       </c>
       <c r="R4" s="3">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Changed tresparametros to D-Station. Strain/Strain Rate files are now found automatically!
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -707,13 +707,13 @@
         <v>382</v>
       </c>
       <c r="G4" s="13" t="n">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H4" s="13" t="n">
-        <v>1145</v>
+        <v>1140</v>
       </c>
       <c r="I4" s="13" t="n">
-        <v>1012</v>
+        <v>1037</v>
       </c>
       <c r="J4" s="16" t="n">
         <v>1101</v>
@@ -740,7 +740,7 @@
         <v/>
       </c>
       <c r="Q4" s="13" t="n">
-        <v>734</v>
+        <v>700</v>
       </c>
       <c r="R4" s="13">
         <f>J4-I4</f>

</xml_diff>

<commit_message>
Strain rate can now be obtained from Strain curves/Option added
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -690,13 +690,13 @@
         <v>382</v>
       </c>
       <c r="G4" s="17" t="n">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H4" s="17" t="n">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="I4" s="17" t="n">
-        <v>1025</v>
+        <v>1028</v>
       </c>
       <c r="J4" s="18" t="n"/>
       <c r="K4" s="19" t="n"/>

</xml_diff>

<commit_message>
IVRT changed to IVR
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -690,13 +690,13 @@
         <v>382</v>
       </c>
       <c r="G4" s="17" t="n">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H4" s="17" t="n">
-        <v>1144</v>
+        <v>1107</v>
       </c>
       <c r="I4" s="17" t="n">
-        <v>1028</v>
+        <v>1035</v>
       </c>
       <c r="J4" s="18" t="n"/>
       <c r="K4" s="19" t="n"/>

</xml_diff>

<commit_message>
Patients are now registered in Event_Timing.
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
@@ -16,14 +15,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
-  <si>
-    <t>pontos marcados</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+  <si>
+    <t>Pontos marcados</t>
   </si>
   <si>
     <t>IdPatient</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>MVO</t>
   </si>
   <si>
@@ -48,25 +50,16 @@
     <t>Aristoteles</t>
   </si>
   <si>
-    <t>Electrical Mechanical Coupling = Onset QRS – MVC (Troquei a ordem)</t>
-  </si>
-  <si>
-    <t>IVC = AVO - MVC</t>
-  </si>
-  <si>
-    <t>Eject = AVC – AVO</t>
-  </si>
-  <si>
-    <t>Isovolumetric Relaxation Time = MVO – AVC</t>
-  </si>
-  <si>
-    <t>Early Filling Phase = Onset P Wave – MVO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Late Filling Phase = </t>
-  </si>
-  <si>
-    <t>Atrial Contraction = P wave peak – P wave onset</t>
+    <t>Adilson</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Yamaguchi</t>
+  </si>
+  <si>
+    <t>Teste1</t>
   </si>
 </sst>
 </file>
@@ -74,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -101,12 +94,6 @@
       <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="16"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -176,7 +163,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -186,29 +173,23 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
@@ -217,29 +198,23 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -542,191 +517,279 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
-      <selection activeCell="B16" activeCellId="0" pane="topLeft" sqref="B16"/>
+      <selection activeCell="B21" activeCellId="0" pane="topLeft" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="11" width="28.21"/>
-    <col customWidth="1" max="2" min="2" style="11" width="44.89"/>
-    <col customWidth="1" max="3" min="3" style="11" width="17.1"/>
-    <col customWidth="1" max="4" min="4" style="11" width="15.61"/>
-    <col customWidth="1" max="5" min="5" style="11" width="15.39"/>
-    <col customWidth="1" max="6" min="6" style="11" width="17.1"/>
-    <col customWidth="1" max="7" min="7" style="11" width="19.84"/>
-    <col customWidth="1" max="8" min="8" style="11" width="21.06"/>
-    <col customWidth="1" max="9" min="9" style="11" width="26.51"/>
-    <col customWidth="1" max="10" min="10" style="11" width="23.3"/>
-    <col customWidth="1" max="11" min="11" style="11" width="17.55"/>
-    <col customWidth="1" max="12" min="12" style="11" width="24.41"/>
-    <col customWidth="1" max="13" min="13" style="11" width="13.09"/>
-    <col customWidth="1" max="14" min="14" style="11" width="22.95"/>
-    <col customWidth="1" max="15" min="15" style="11" width="17.28"/>
-    <col customWidth="1" max="16" min="16" style="11" width="14.58"/>
-    <col customWidth="1" max="18" min="17" style="11" width="15.53"/>
-    <col customWidth="1" max="1025" min="19" style="11" width="9.85"/>
+    <col customWidth="1" max="1" min="1" style="9" width="28.21"/>
+    <col customWidth="1" max="2" min="2" style="9" width="44.89"/>
+    <col customWidth="1" max="3" min="3" style="9" width="17.1"/>
+    <col customWidth="1" max="4" min="4" style="9" width="15.61"/>
+    <col customWidth="1" max="5" min="5" style="9" width="15.39"/>
+    <col customWidth="1" max="6" min="6" style="9" width="17.1"/>
+    <col customWidth="1" max="7" min="7" style="9" width="19.84"/>
+    <col customWidth="1" max="8" min="8" style="9" width="21.06"/>
+    <col customWidth="1" max="9" min="9" style="9" width="26.51"/>
+    <col customWidth="1" max="10" min="10" style="9" width="23.3"/>
+    <col customWidth="1" max="11" min="11" style="9" width="17.55"/>
+    <col customWidth="1" max="12" min="12" style="9" width="24.41"/>
+    <col customWidth="1" max="13" min="13" style="9" width="13.09"/>
+    <col customWidth="1" max="14" min="14" style="9" width="22.95"/>
+    <col customWidth="1" max="15" min="15" style="9" width="17.28"/>
+    <col customWidth="1" max="16" min="16" style="9" width="14.58"/>
+    <col customWidth="1" max="18" min="17" style="9" width="15.53"/>
+    <col customWidth="1" max="1025" min="19" style="9" width="9.85"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.8" r="1" s="12" spans="1:26">
-      <c r="A1" s="13" t="n"/>
-      <c r="B1" s="13" t="n"/>
-      <c r="C1" s="13" t="n"/>
-      <c r="D1" s="13" t="n"/>
-      <c r="E1" s="13" t="n"/>
-      <c r="F1" s="13" t="n"/>
-      <c r="G1" s="13" t="n"/>
-      <c r="H1" s="14" t="s">
+    <row customHeight="1" ht="12.8" r="1" s="10" spans="1:26">
+      <c r="A1" s="11" t="n"/>
+      <c r="B1" s="11" t="n"/>
+      <c r="C1" s="11" t="n"/>
+      <c r="D1" s="11" t="n"/>
+      <c r="E1" s="11" t="n"/>
+      <c r="F1" s="11" t="n"/>
+      <c r="G1" s="12" t="n"/>
+      <c r="H1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="13" t="n"/>
-      <c r="J1" s="13" t="n"/>
-      <c r="K1" s="13" t="n"/>
-      <c r="L1" s="13" t="n"/>
-      <c r="M1" s="13" t="n"/>
-      <c r="N1" s="13" t="n"/>
-      <c r="O1" s="13" t="n"/>
-      <c r="P1" s="13" t="n"/>
-      <c r="Q1" s="13" t="n"/>
-      <c r="R1" s="13" t="n"/>
-      <c r="S1" s="13" t="n"/>
-      <c r="T1" s="13" t="n"/>
-      <c r="U1" s="13" t="n"/>
-      <c r="V1" s="13" t="n"/>
-      <c r="W1" s="13" t="n"/>
-      <c r="X1" s="13" t="n"/>
-      <c r="Y1" s="13" t="n"/>
-      <c r="Z1" s="13" t="n"/>
+      <c r="I1" s="12" t="n"/>
+      <c r="J1" s="11" t="n"/>
+      <c r="K1" s="11" t="n"/>
+      <c r="L1" s="11" t="n"/>
+      <c r="M1" s="11" t="n"/>
+      <c r="N1" s="11" t="n"/>
+      <c r="O1" s="11" t="n"/>
+      <c r="P1" s="11" t="n"/>
+      <c r="Q1" s="11" t="n"/>
+      <c r="R1" s="11" t="n"/>
+      <c r="S1" s="11" t="n"/>
+      <c r="T1" s="11" t="n"/>
+      <c r="U1" s="11" t="n"/>
+      <c r="V1" s="11" t="n"/>
+      <c r="W1" s="11" t="n"/>
+      <c r="X1" s="11" t="n"/>
+      <c r="Y1" s="11" t="n"/>
+      <c r="Z1" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="19.7" r="2" s="12" spans="1:26">
-      <c r="A2" s="15" t="s">
+    <row customHeight="1" ht="19.7" r="2" s="10" spans="1:26">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="n"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="15" t="n"/>
-      <c r="K2" s="15" t="n"/>
-      <c r="L2" s="16" t="n"/>
-      <c r="M2" s="16" t="n"/>
-      <c r="N2" s="16" t="n"/>
-      <c r="O2" s="16" t="n"/>
-      <c r="P2" s="16" t="n"/>
-      <c r="Q2" s="16" t="n"/>
-      <c r="R2" s="16" t="n"/>
-      <c r="S2" s="13" t="n"/>
-      <c r="T2" s="13" t="n"/>
-      <c r="U2" s="13" t="n"/>
-      <c r="V2" s="13" t="n"/>
-      <c r="W2" s="13" t="n"/>
-      <c r="X2" s="13" t="n"/>
-      <c r="Y2" s="13" t="n"/>
-      <c r="Z2" s="13" t="n"/>
+      <c r="I2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="12" t="n"/>
+      <c r="K2" s="12" t="n"/>
+      <c r="L2" s="13" t="n"/>
+      <c r="M2" s="13" t="n"/>
+      <c r="N2" s="13" t="n"/>
+      <c r="O2" s="13" t="n"/>
+      <c r="P2" s="13" t="n"/>
+      <c r="Q2" s="13" t="n"/>
+      <c r="R2" s="13" t="n"/>
+      <c r="S2" s="11" t="n"/>
+      <c r="T2" s="11" t="n"/>
+      <c r="U2" s="11" t="n"/>
+      <c r="V2" s="11" t="n"/>
+      <c r="W2" s="11" t="n"/>
+      <c r="X2" s="11" t="n"/>
+      <c r="Y2" s="11" t="n"/>
+      <c r="Z2" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="3" s="12" spans="1:26">
-      <c r="A3" s="17" t="n"/>
-      <c r="B3" s="17" t="n"/>
-      <c r="C3" s="17" t="n"/>
-      <c r="D3" s="17" t="n"/>
-      <c r="E3" s="17" t="n"/>
-      <c r="F3" s="17" t="n"/>
-      <c r="G3" s="17" t="n"/>
-      <c r="H3" s="17" t="n"/>
-      <c r="I3" s="17" t="n"/>
-      <c r="J3" s="18" t="n"/>
-      <c r="K3" s="18" t="n"/>
-      <c r="L3" s="17" t="n"/>
-      <c r="M3" s="17" t="n"/>
-      <c r="N3" s="17" t="n"/>
-      <c r="O3" s="17" t="n"/>
-      <c r="P3" s="17" t="n"/>
-      <c r="Q3" s="17" t="n"/>
-      <c r="R3" s="17" t="n"/>
-      <c r="S3" s="13" t="n"/>
-      <c r="T3" s="13" t="n"/>
-      <c r="U3" s="13" t="n"/>
-      <c r="V3" s="13" t="n"/>
-      <c r="W3" s="13" t="n"/>
-      <c r="X3" s="13" t="n"/>
-      <c r="Y3" s="13" t="n"/>
-      <c r="Z3" s="13" t="n"/>
+    <row customHeight="1" ht="15" r="3" s="10" spans="1:26">
+      <c r="A3" s="14" t="n"/>
+      <c r="B3" s="14" t="n"/>
+      <c r="C3" s="14" t="n"/>
+      <c r="D3" s="14" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="14" t="n"/>
+      <c r="G3" s="14" t="n"/>
+      <c r="H3" s="14" t="n"/>
+      <c r="I3" s="14" t="n"/>
+      <c r="J3" s="15" t="n"/>
+      <c r="K3" s="15" t="n"/>
+      <c r="L3" s="14" t="n"/>
+      <c r="M3" s="14" t="n"/>
+      <c r="N3" s="14" t="n"/>
+      <c r="O3" s="14" t="n"/>
+      <c r="P3" s="14" t="n"/>
+      <c r="Q3" s="14" t="n"/>
+      <c r="R3" s="14" t="n"/>
+      <c r="S3" s="11" t="n"/>
+      <c r="T3" s="11" t="n"/>
+      <c r="U3" s="11" t="n"/>
+      <c r="V3" s="11" t="n"/>
+      <c r="W3" s="11" t="n"/>
+      <c r="X3" s="11" t="n"/>
+      <c r="Y3" s="11" t="n"/>
+      <c r="Z3" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4" s="12" spans="1:26">
-      <c r="A4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="17" t="n"/>
-      <c r="C4" s="17" t="n">
+    <row customHeight="1" ht="15" r="4" s="10" spans="1:26">
+      <c r="A4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="14" t="n"/>
+      <c r="C4" s="14" t="n">
         <v>453</v>
       </c>
-      <c r="D4" s="17" t="n">
+      <c r="D4" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="E4" s="17" t="n">
+      <c r="E4" s="14" t="n">
         <v>72</v>
       </c>
-      <c r="F4" s="17" t="n">
+      <c r="F4" s="14" t="n">
         <v>382</v>
       </c>
-      <c r="G4" s="17" t="n">
-        <v>102</v>
-      </c>
-      <c r="H4" s="17" t="n">
-        <v>1108</v>
-      </c>
-      <c r="I4" s="17" t="n">
-        <v>1031</v>
-      </c>
-      <c r="J4" s="18" t="n"/>
-      <c r="K4" s="19" t="n"/>
-      <c r="L4" s="17" t="n"/>
-      <c r="M4" s="17" t="n"/>
-      <c r="N4" s="17" t="n"/>
-      <c r="O4" s="17" t="n"/>
-      <c r="P4" s="17" t="n"/>
-      <c r="Q4" s="17" t="n"/>
-      <c r="R4" s="17" t="n"/>
-      <c r="S4" s="20" t="n"/>
-      <c r="T4" s="20" t="n"/>
-      <c r="U4" s="13" t="n"/>
-      <c r="V4" s="13" t="n"/>
-      <c r="W4" s="13" t="n"/>
-      <c r="X4" s="13" t="n"/>
-      <c r="Y4" s="13" t="n"/>
-      <c r="Z4" s="13" t="n"/>
+      <c r="G4" s="14" t="n">
+        <v>105</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>1139</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <v>1029</v>
+      </c>
+      <c r="J4" s="15" t="n"/>
+      <c r="K4" s="16" t="n"/>
+      <c r="L4" s="14" t="n"/>
+      <c r="M4" s="14" t="n"/>
+      <c r="N4" s="14" t="n"/>
+      <c r="O4" s="14" t="n"/>
+      <c r="P4" s="14" t="n"/>
+      <c r="Q4" s="14" t="n"/>
+      <c r="R4" s="14" t="n"/>
+      <c r="S4" s="17" t="n"/>
+      <c r="T4" s="17" t="n"/>
+      <c r="U4" s="11" t="n"/>
+      <c r="V4" s="11" t="n"/>
+      <c r="W4" s="11" t="n"/>
+      <c r="X4" s="11" t="n"/>
+      <c r="Y4" s="11" t="n"/>
+      <c r="Z4" s="11" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="6" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="7" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="8" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="9" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="10" s="12" spans="1:26"/>
-    <row customHeight="1" ht="19.7" r="13" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="14" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="15" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="21" s="12" spans="1:26"/>
-    <row customHeight="1" ht="15" r="22" s="12" spans="1:26"/>
+    <row customHeight="1" ht="15" r="5" s="10" spans="1:26">
+      <c r="A5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14" t="n"/>
+      <c r="C5" s="14" t="n">
+        <v>609</v>
+      </c>
+      <c r="D5" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <v>126</v>
+      </c>
+      <c r="F5" s="14" t="n">
+        <v>428</v>
+      </c>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="14" t="n"/>
+      <c r="I5" s="14" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="6" s="10" spans="1:26">
+      <c r="A6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14" t="n"/>
+      <c r="C6" s="14" t="n">
+        <v>525</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>37</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <v>152</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>441</v>
+      </c>
+      <c r="G6" s="14" t="n">
+        <v>40</v>
+      </c>
+      <c r="H6" s="14" t="n">
+        <v>1080</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <v>969</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="7" s="10" spans="1:26">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="14" t="n"/>
+      <c r="C7" s="14" t="n">
+        <v>404</v>
+      </c>
+      <c r="D7" s="14" t="n">
+        <v>823</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>61</v>
+      </c>
+      <c r="F7" s="14" t="n">
+        <v>310</v>
+      </c>
+      <c r="G7" s="14" t="n"/>
+      <c r="H7" s="14" t="n"/>
+      <c r="I7" s="14" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="8" s="10" spans="1:26">
+      <c r="A8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="14" t="n"/>
+      <c r="C8" s="14" t="n">
+        <v>654.5</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>272.8</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>336</v>
+      </c>
+      <c r="F8" s="14" t="n">
+        <v>586.034402</v>
+      </c>
+      <c r="G8" s="14" t="n"/>
+      <c r="H8" s="14" t="n"/>
+      <c r="I8" s="14" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="9" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="10" s="10" spans="1:26"/>
+    <row customHeight="1" ht="19.7" r="13" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="14" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="15" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="21" s="10" spans="1:26"/>
+    <row customHeight="1" ht="15" r="22" s="10" spans="1:26"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="1" verticalCentered="1"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
@@ -740,71 +803,4 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="B4:B17"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E17" activeCellId="0" pane="topLeft" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1025" min="1" style="21" width="10.12"/>
-  </cols>
-  <sheetData>
-    <row customHeight="1" ht="12.8" r="4" s="12" spans="1:2">
-      <c r="B4" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="6" s="12" spans="1:2">
-      <c r="B6" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="9" s="12" spans="1:2">
-      <c r="B9" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="11" s="12" spans="1:2">
-      <c r="B11" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="13" s="12" spans="1:2">
-      <c r="B13" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="15" s="12" spans="1:2">
-      <c r="B15" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="17" s="12" spans="1:2">
-      <c r="B17" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-  <headerFooter differentFirst="0" differentOddEven="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Parameters are now calculated at the same time.
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -667,13 +667,13 @@
         <v>382</v>
       </c>
       <c r="G4" s="14" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H4" s="14" t="n">
-        <v>1139</v>
+        <v>1149</v>
       </c>
       <c r="I4" s="14" t="n">
-        <v>1029</v>
+        <v>1014</v>
       </c>
       <c r="J4" s="15" t="n"/>
       <c r="K4" s="16" t="n"/>

</xml_diff>

<commit_message>
Comments about future updates added.
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -667,13 +667,13 @@
         <v>382</v>
       </c>
       <c r="G4" s="14" t="n">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H4" s="14" t="n">
-        <v>1149</v>
+        <v>1141</v>
       </c>
       <c r="I4" s="14" t="n">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="J4" s="15" t="n"/>
       <c r="K4" s="16" t="n"/>

</xml_diff>

<commit_message>
added ddof = 1 in np.std
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Pontos marcados</t>
   </si>
@@ -93,6 +93,60 @@
   </si>
   <si>
     <t>MariaBento</t>
+  </si>
+  <si>
+    <t>FatimaAparecida</t>
+  </si>
+  <si>
+    <t>MarliRosa</t>
+  </si>
+  <si>
+    <t>JoseMacedo</t>
+  </si>
+  <si>
+    <t>SEMTEMPOS</t>
+  </si>
+  <si>
+    <t>FabricioLucena</t>
+  </si>
+  <si>
+    <t>Neusa</t>
+  </si>
+  <si>
+    <t>Eliene</t>
+  </si>
+  <si>
+    <t>Adauto</t>
+  </si>
+  <si>
+    <t>JoseSilva</t>
+  </si>
+  <si>
+    <t>Diogenes</t>
+  </si>
+  <si>
+    <t>MariaSilva</t>
+  </si>
+  <si>
+    <t>MarcoAntonio</t>
+  </si>
+  <si>
+    <t>Marlene</t>
+  </si>
+  <si>
+    <t>Valdir</t>
+  </si>
+  <si>
+    <t>PedroFernandes</t>
+  </si>
+  <si>
+    <t>MariaNogueira</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Roseli</t>
   </si>
 </sst>
 </file>
@@ -553,10 +607,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
-      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
+      <selection activeCell="B25" activeCellId="0" pane="topLeft" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -708,19 +762,19 @@
         <v>382</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>1144</v>
+        <v>1149</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>1034</v>
+        <v>961</v>
       </c>
       <c r="J4" s="17" t="n">
-        <v>-17.83</v>
+        <v>-16.94</v>
       </c>
       <c r="K4" s="17" t="n">
-        <v>37.29</v>
+        <v>51.55</v>
       </c>
       <c r="L4" s="15" t="n"/>
       <c r="M4" s="15" t="n"/>
@@ -833,8 +887,12 @@
       <c r="G8" s="15" t="n"/>
       <c r="H8" s="15" t="n"/>
       <c r="I8" s="15" t="n"/>
-      <c r="J8" s="17" t="n"/>
-      <c r="K8" s="17" t="n"/>
+      <c r="J8" s="17" t="n">
+        <v>-12.58</v>
+      </c>
+      <c r="K8" s="17" t="n">
+        <v>140.33</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="9" s="11" spans="1:26">
       <c r="A9" s="15" t="s">
@@ -920,19 +978,19 @@
         <v>286</v>
       </c>
       <c r="G11" s="15" t="n">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="H11" s="15" t="n">
-        <v>791</v>
+        <v>754</v>
       </c>
       <c r="I11" s="15" t="n">
-        <v>747</v>
+        <v>693</v>
       </c>
       <c r="J11" s="17" t="n">
-        <v>-4.11</v>
+        <v>-4.18</v>
       </c>
       <c r="K11" s="17" t="n">
-        <v>89.23</v>
+        <v>91.81999999999999</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12" s="11" spans="1:26">
@@ -1100,12 +1158,649 @@
         <v>100.27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17" s="11" spans="1:26"/>
-    <row customHeight="1" ht="15" r="18" s="11" spans="1:26"/>
-    <row customHeight="1" ht="15" r="19" s="11" spans="1:26"/>
-    <row customHeight="1" ht="15" r="20" s="11" spans="1:26"/>
-    <row customHeight="1" ht="15" r="21" s="11" spans="1:26"/>
-    <row customHeight="1" ht="15" r="22" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="17" s="11" spans="1:26">
+      <c r="A17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="17" t="n"/>
+      <c r="C17" s="17" t="n">
+        <v>451</v>
+      </c>
+      <c r="D17" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="E17" s="17" t="n">
+        <v>67</v>
+      </c>
+      <c r="F17" s="17" t="n">
+        <v>374</v>
+      </c>
+      <c r="G17" s="17" t="n">
+        <v>67</v>
+      </c>
+      <c r="H17" s="17" t="n">
+        <v>883</v>
+      </c>
+      <c r="I17" s="17" t="n">
+        <v>782</v>
+      </c>
+      <c r="J17" s="17" t="n">
+        <v>-17.01</v>
+      </c>
+      <c r="K17" s="17" t="n">
+        <v>37.28</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="18" s="11" spans="1:26">
+      <c r="A18" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="17" t="n"/>
+      <c r="C18" s="17" t="n">
+        <v>493</v>
+      </c>
+      <c r="D18" s="17" t="n">
+        <v>905</v>
+      </c>
+      <c r="E18" s="17" t="n">
+        <v>46</v>
+      </c>
+      <c r="F18" s="17" t="n">
+        <v>384</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>35</v>
+      </c>
+      <c r="H18" s="17" t="n">
+        <v>938</v>
+      </c>
+      <c r="I18" s="17" t="n">
+        <v>840</v>
+      </c>
+      <c r="J18" s="17" t="n">
+        <v>-20.02</v>
+      </c>
+      <c r="K18" s="17" t="n">
+        <v>41.47</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="19" s="11" spans="1:26">
+      <c r="A19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="17" t="n"/>
+      <c r="C19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="17" t="n"/>
+      <c r="E19" s="17" t="n"/>
+      <c r="F19" s="17" t="n"/>
+      <c r="G19" s="17" t="n"/>
+      <c r="H19" s="17" t="n"/>
+      <c r="I19" s="17" t="n"/>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="20" s="11" spans="1:26">
+      <c r="A20" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="17" t="n">
+        <v>397</v>
+      </c>
+      <c r="D20" s="17" t="n">
+        <v>877</v>
+      </c>
+      <c r="E20" s="17" t="n">
+        <v>65</v>
+      </c>
+      <c r="F20" s="17" t="n">
+        <v>326</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <v>48</v>
+      </c>
+      <c r="H20" s="17" t="n">
+        <v>942</v>
+      </c>
+      <c r="I20" s="17" t="n">
+        <v>835</v>
+      </c>
+      <c r="J20" s="17" t="n">
+        <v>-19.29</v>
+      </c>
+      <c r="K20" s="17" t="n">
+        <v>37.97</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="21" s="11" spans="1:26">
+      <c r="A21" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="17" t="n"/>
+      <c r="C21" s="17" t="n">
+        <v>515</v>
+      </c>
+      <c r="D21" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="E21" s="17" t="n">
+        <v>31</v>
+      </c>
+      <c r="F21" s="17" t="n">
+        <v>385</v>
+      </c>
+      <c r="G21" s="17" t="n">
+        <v>119</v>
+      </c>
+      <c r="H21" s="17" t="n">
+        <v>1216</v>
+      </c>
+      <c r="I21" s="17" t="n">
+        <v>1113</v>
+      </c>
+      <c r="J21" s="17" t="n">
+        <v>-15.15</v>
+      </c>
+      <c r="K21" s="17" t="n">
+        <v>69.8</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="11" spans="1:26">
+      <c r="A22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="17" t="n"/>
+      <c r="C22" s="17" t="n">
+        <v>484</v>
+      </c>
+      <c r="D22" s="17" t="n">
+        <v>1071</v>
+      </c>
+      <c r="E22" s="17" t="n">
+        <v>78</v>
+      </c>
+      <c r="F22" s="17" t="n">
+        <v>396</v>
+      </c>
+      <c r="G22" s="17" t="n">
+        <v>22</v>
+      </c>
+      <c r="H22" s="17" t="n">
+        <v>1014</v>
+      </c>
+      <c r="I22" s="17" t="n">
+        <v>784</v>
+      </c>
+      <c r="J22" s="17" t="n">
+        <v>-16.42</v>
+      </c>
+      <c r="K22" s="17" t="n">
+        <v>89.34</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="23" s="11" spans="1:26">
+      <c r="A23" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="17" t="n"/>
+      <c r="C23" s="17" t="n">
+        <v>561</v>
+      </c>
+      <c r="D23" s="17" t="n">
+        <v>45</v>
+      </c>
+      <c r="E23" s="17" t="n">
+        <v>68</v>
+      </c>
+      <c r="F23" s="17" t="n">
+        <v>412</v>
+      </c>
+      <c r="G23" s="17" t="n">
+        <v>119</v>
+      </c>
+      <c r="H23" s="17" t="n">
+        <v>1255</v>
+      </c>
+      <c r="I23" s="17" t="n">
+        <v>1099</v>
+      </c>
+      <c r="J23" s="17" t="n">
+        <v>-18.99</v>
+      </c>
+      <c r="K23" s="17" t="n">
+        <v>49.95</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="11" spans="1:26">
+      <c r="A24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="17" t="n"/>
+      <c r="C24" s="17" t="n">
+        <v>453</v>
+      </c>
+      <c r="D24" s="17" t="n">
+        <v>924</v>
+      </c>
+      <c r="E24" s="17" t="n">
+        <v>49</v>
+      </c>
+      <c r="F24" s="17" t="n">
+        <v>355</v>
+      </c>
+      <c r="G24" s="17" t="n">
+        <v>140</v>
+      </c>
+      <c r="H24" s="17" t="n">
+        <v>1153</v>
+      </c>
+      <c r="I24" s="17" t="n">
+        <v>950</v>
+      </c>
+      <c r="J24" s="17" t="n">
+        <v>-16.81</v>
+      </c>
+      <c r="K24" s="17" t="n">
+        <v>51.55</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="25" s="11" spans="1:26">
+      <c r="A25" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="17" t="n"/>
+      <c r="C25" s="17" t="n">
+        <v>399</v>
+      </c>
+      <c r="D25" s="17" t="n">
+        <v>796</v>
+      </c>
+      <c r="E25" s="17" t="n">
+        <v>74</v>
+      </c>
+      <c r="F25" s="17" t="n">
+        <v>354</v>
+      </c>
+      <c r="G25" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="H25" s="17" t="n">
+        <v>1162</v>
+      </c>
+      <c r="I25" s="17" t="n">
+        <v>1043</v>
+      </c>
+      <c r="J25" s="17" t="n">
+        <v>-10.3</v>
+      </c>
+      <c r="K25" s="17" t="n">
+        <v>96.77</v>
+      </c>
+      <c r="L25" s="17" t="n"/>
+      <c r="M25" s="17" t="n"/>
+      <c r="N25" s="17" t="n"/>
+      <c r="O25" s="17" t="n"/>
+      <c r="P25" s="17" t="n"/>
+      <c r="Q25" s="17" t="n"/>
+      <c r="R25" s="17" t="n"/>
+      <c r="S25" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="26" s="11" spans="1:26">
+      <c r="A26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="17" t="n"/>
+      <c r="C26" s="17" t="n">
+        <v>548</v>
+      </c>
+      <c r="D26" s="17" t="n">
+        <v>55</v>
+      </c>
+      <c r="E26" s="17" t="n">
+        <v>78</v>
+      </c>
+      <c r="F26" s="17" t="n">
+        <v>409</v>
+      </c>
+      <c r="G26" s="17" t="n">
+        <v>115</v>
+      </c>
+      <c r="H26" s="17" t="n">
+        <v>1280</v>
+      </c>
+      <c r="I26" s="17" t="n">
+        <v>1194</v>
+      </c>
+      <c r="J26" s="17" t="n">
+        <v>-19.84</v>
+      </c>
+      <c r="K26" s="17" t="n">
+        <v>36.86</v>
+      </c>
+      <c r="L26" s="17" t="n"/>
+      <c r="M26" s="17" t="n"/>
+      <c r="N26" s="17" t="n"/>
+      <c r="O26" s="17" t="n"/>
+      <c r="P26" s="17" t="n"/>
+      <c r="Q26" s="17" t="n"/>
+      <c r="R26" s="17" t="n"/>
+      <c r="S26" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="27" s="11" spans="1:26">
+      <c r="A27" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="17" t="n"/>
+      <c r="C27" s="17" t="n">
+        <v>730</v>
+      </c>
+      <c r="D27" s="17" t="n">
+        <v>1011</v>
+      </c>
+      <c r="E27" s="17" t="n">
+        <v>1085</v>
+      </c>
+      <c r="F27" s="17" t="n">
+        <v>1333</v>
+      </c>
+      <c r="G27" s="17" t="n"/>
+      <c r="H27" s="17" t="n"/>
+      <c r="I27" s="17" t="n"/>
+      <c r="J27" s="17" t="n"/>
+      <c r="K27" s="17" t="n"/>
+      <c r="L27" s="17" t="n"/>
+      <c r="M27" s="17" t="n"/>
+      <c r="N27" s="17" t="n"/>
+      <c r="O27" s="17" t="n"/>
+      <c r="P27" s="17" t="n"/>
+      <c r="Q27" s="17" t="n"/>
+      <c r="R27" s="17" t="n"/>
+      <c r="S27" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="28" s="11" spans="1:26">
+      <c r="A28" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="17" t="n"/>
+      <c r="C28" s="17" t="n">
+        <v>493</v>
+      </c>
+      <c r="D28" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E28" s="17" t="n">
+        <v>63</v>
+      </c>
+      <c r="F28" s="17" t="n">
+        <v>425</v>
+      </c>
+      <c r="G28" s="17" t="n">
+        <v>35</v>
+      </c>
+      <c r="H28" s="17" t="n">
+        <v>939</v>
+      </c>
+      <c r="I28" s="17" t="n">
+        <v>851</v>
+      </c>
+      <c r="J28" s="17" t="n">
+        <v>-20.9</v>
+      </c>
+      <c r="K28" s="17" t="n">
+        <v>132.72</v>
+      </c>
+      <c r="L28" s="17" t="n"/>
+      <c r="M28" s="17" t="n"/>
+      <c r="N28" s="17" t="n"/>
+      <c r="O28" s="17" t="n"/>
+      <c r="P28" s="17" t="n"/>
+      <c r="Q28" s="17" t="n"/>
+      <c r="R28" s="17" t="n"/>
+      <c r="S28" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="29" s="11" spans="1:26">
+      <c r="A29" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="17" t="n"/>
+      <c r="C29" s="17" t="n">
+        <v>422</v>
+      </c>
+      <c r="D29" s="17" t="n">
+        <v>840</v>
+      </c>
+      <c r="E29" s="17" t="n">
+        <v>38</v>
+      </c>
+      <c r="F29" s="17" t="n">
+        <v>331</v>
+      </c>
+      <c r="G29" s="17" t="n">
+        <v>101</v>
+      </c>
+      <c r="H29" s="17" t="n">
+        <v>1019</v>
+      </c>
+      <c r="I29" s="17" t="n">
+        <v>954</v>
+      </c>
+      <c r="J29" s="17" t="n">
+        <v>-15.04</v>
+      </c>
+      <c r="K29" s="17" t="n">
+        <v>82.59</v>
+      </c>
+      <c r="L29" s="17" t="n"/>
+      <c r="M29" s="17" t="n"/>
+      <c r="N29" s="17" t="n"/>
+      <c r="O29" s="17" t="n"/>
+      <c r="P29" s="17" t="n"/>
+      <c r="Q29" s="17" t="n"/>
+      <c r="R29" s="17" t="n"/>
+      <c r="S29" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="30" s="11" spans="1:26">
+      <c r="A30" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="17" t="n"/>
+      <c r="C30" s="17" t="n">
+        <v>434</v>
+      </c>
+      <c r="D30" s="17" t="n">
+        <v>976</v>
+      </c>
+      <c r="E30" s="17" t="n">
+        <v>40</v>
+      </c>
+      <c r="F30" s="17" t="n">
+        <v>341</v>
+      </c>
+      <c r="G30" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="H30" s="17" t="n">
+        <v>1074</v>
+      </c>
+      <c r="I30" s="17" t="n">
+        <v>871</v>
+      </c>
+      <c r="J30" s="17" t="n">
+        <v>-19.96</v>
+      </c>
+      <c r="K30" s="17" t="n">
+        <v>101.56</v>
+      </c>
+      <c r="L30" s="17" t="n"/>
+      <c r="M30" s="17" t="n"/>
+      <c r="N30" s="17" t="n"/>
+      <c r="O30" s="17" t="n"/>
+      <c r="P30" s="17" t="n"/>
+      <c r="Q30" s="17" t="n"/>
+      <c r="R30" s="17" t="n"/>
+      <c r="S30" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="31" s="11" spans="1:26">
+      <c r="A31" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="17" t="n"/>
+      <c r="C31" s="17" t="n">
+        <v>351</v>
+      </c>
+      <c r="D31" s="17" t="n">
+        <v>26</v>
+      </c>
+      <c r="E31" s="17" t="n">
+        <v>74</v>
+      </c>
+      <c r="F31" s="17" t="n">
+        <v>384</v>
+      </c>
+      <c r="G31" s="17" t="n"/>
+      <c r="H31" s="17" t="n"/>
+      <c r="I31" s="17" t="n"/>
+      <c r="J31" s="17" t="n"/>
+      <c r="K31" s="17" t="n"/>
+      <c r="L31" s="17" t="n"/>
+      <c r="M31" s="17" t="n"/>
+      <c r="N31" s="17" t="n"/>
+      <c r="O31" s="17" t="n"/>
+      <c r="P31" s="17" t="n"/>
+      <c r="Q31" s="17" t="n"/>
+      <c r="R31" s="17" t="n"/>
+      <c r="S31" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="32" s="11" spans="1:26">
+      <c r="A32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="17" t="n"/>
+      <c r="C32" s="17" t="n">
+        <v>445</v>
+      </c>
+      <c r="D32" s="17" t="n">
+        <v>817</v>
+      </c>
+      <c r="E32" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="F32" s="17" t="n">
+        <v>399</v>
+      </c>
+      <c r="G32" s="17" t="n">
+        <v>29</v>
+      </c>
+      <c r="H32" s="17" t="n">
+        <v>837</v>
+      </c>
+      <c r="I32" s="17" t="n">
+        <v>761</v>
+      </c>
+      <c r="J32" s="17" t="n">
+        <v>-20.42</v>
+      </c>
+      <c r="K32" s="17" t="n">
+        <v>53</v>
+      </c>
+      <c r="L32" s="17" t="n"/>
+      <c r="M32" s="17" t="n"/>
+      <c r="N32" s="17" t="n"/>
+      <c r="O32" s="17" t="n"/>
+      <c r="P32" s="17" t="n"/>
+      <c r="Q32" s="17" t="n"/>
+      <c r="R32" s="17" t="n"/>
+      <c r="S32" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="33" s="11" spans="1:26">
+      <c r="A33" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="17" t="n"/>
+      <c r="C33" s="17" t="n">
+        <v>443</v>
+      </c>
+      <c r="D33" s="17" t="n">
+        <v>783</v>
+      </c>
+      <c r="E33" s="17" t="n">
+        <v>61</v>
+      </c>
+      <c r="F33" s="17" t="n">
+        <v>359</v>
+      </c>
+      <c r="G33" s="17" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="17" t="n">
+        <v>698</v>
+      </c>
+      <c r="I33" s="17" t="n">
+        <v>610</v>
+      </c>
+      <c r="J33" s="17" t="n">
+        <v>-17.96</v>
+      </c>
+      <c r="K33" s="17" t="n">
+        <v>150.33</v>
+      </c>
+      <c r="L33" s="17" t="n"/>
+      <c r="M33" s="17" t="n"/>
+      <c r="N33" s="17" t="n"/>
+      <c r="O33" s="17" t="n"/>
+      <c r="P33" s="17" t="n"/>
+      <c r="Q33" s="17" t="n"/>
+      <c r="R33" s="17" t="n"/>
+      <c r="S33" s="17" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="34" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="35" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="36" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="37" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="38" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="39" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="40" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="41" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="42" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="43" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="44" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="45" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="46" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="47" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="48" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="49" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="50" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="51" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="52" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="53" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="54" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="55" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="56" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="57" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="58" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="59" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="60" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="61" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="62" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="63" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="64" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="65" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="66" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="67" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="68" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="69" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="70" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="71" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="72" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="73" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="74" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="75" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="76" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="77" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="78" s="11" spans="1:26"/>
+    <row customHeight="1" ht="15" r="79" s="11" spans="1:26"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>

</xml_diff>

<commit_message>
Fontsize is now defined by constant
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -762,19 +762,19 @@
         <v>382</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>961</v>
+        <v>1028</v>
       </c>
       <c r="J4" s="17" t="n">
-        <v>-16.94</v>
+        <v>-17.83</v>
       </c>
       <c r="K4" s="17" t="n">
-        <v>51.55</v>
+        <v>38.37</v>
       </c>
       <c r="L4" s="15" t="n"/>
       <c r="M4" s="15" t="n"/>
@@ -891,7 +891,7 @@
         <v>-12.58</v>
       </c>
       <c r="K8" s="17" t="n">
-        <v>140.33</v>
+        <v>144.93</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="9" s="11" spans="1:26">

</xml_diff>

<commit_message>
GLS corrected. Must find the MD errors and sync all of the 16 curves.
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -666,8 +666,8 @@
   </sheetPr>
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
-      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="C25" activeCellId="0" pane="topLeft" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -849,40 +849,40 @@
         <v>382</v>
       </c>
       <c r="G4" s="20" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H4" s="20" t="n">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="I4" s="20" t="n">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="J4" s="22" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K4" s="22" t="n">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="L4" s="20" t="n">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="M4" s="20" t="n">
-        <v>568</v>
+        <v>581</v>
       </c>
       <c r="N4" s="20" t="n">
-        <v>639</v>
+        <v>652</v>
       </c>
       <c r="O4" s="20" t="n">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="P4" s="20" t="n">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="Q4" s="20" t="n">
-        <v>1166</v>
+        <v>1246</v>
       </c>
       <c r="R4" s="20" t="n">
-        <v>1214</v>
+        <v>1294</v>
       </c>
       <c r="S4" s="22" t="n">
         <v>358</v>
@@ -1179,28 +1179,46 @@
         <v>286</v>
       </c>
       <c r="G11" s="20" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" s="20" t="n">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="I11" s="20" t="n">
-        <v>693</v>
-      </c>
-      <c r="J11" s="22" t="n"/>
-      <c r="K11" s="22" t="n"/>
-      <c r="L11" s="24" t="n"/>
-      <c r="M11" s="24" t="n"/>
-      <c r="N11" s="24" t="n"/>
-      <c r="O11" s="24" t="n"/>
-      <c r="P11" s="24" t="n"/>
-      <c r="Q11" s="24" t="n"/>
-      <c r="R11" s="24" t="n"/>
+        <v>682</v>
+      </c>
+      <c r="J11" s="22" t="n">
+        <v>54</v>
+      </c>
+      <c r="K11" s="22" t="n">
+        <v>808</v>
+      </c>
+      <c r="L11" s="24" t="n">
+        <v>225</v>
+      </c>
+      <c r="M11" s="24" t="n">
+        <v>420</v>
+      </c>
+      <c r="N11" s="24" t="n">
+        <v>517</v>
+      </c>
+      <c r="O11" s="24" t="n">
+        <v>682</v>
+      </c>
+      <c r="P11" s="24" t="n">
+        <v>758</v>
+      </c>
+      <c r="Q11" s="24" t="n">
+        <v>1491</v>
+      </c>
+      <c r="R11" s="24" t="n">
+        <v>908</v>
+      </c>
       <c r="S11" s="22" t="n"/>
       <c r="T11" s="22" t="n"/>
       <c r="U11" s="24" t="n"/>
       <c r="V11" s="24" t="n">
-        <v>-4.18</v>
+        <v>-4.4</v>
       </c>
       <c r="W11" s="24" t="n">
         <v>91.81999999999999</v>
@@ -1269,31 +1287,49 @@
         <v>375</v>
       </c>
       <c r="G13" s="20" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H13" s="20" t="n">
-        <v>1035</v>
+        <v>1041</v>
       </c>
       <c r="I13" s="20" t="n">
-        <v>951</v>
-      </c>
-      <c r="J13" s="22" t="n"/>
-      <c r="K13" s="22" t="n"/>
-      <c r="L13" s="24" t="n"/>
-      <c r="M13" s="24" t="n"/>
-      <c r="N13" s="24" t="n"/>
-      <c r="O13" s="24" t="n"/>
-      <c r="P13" s="24" t="n"/>
-      <c r="Q13" s="24" t="n"/>
-      <c r="R13" s="24" t="n"/>
+        <v>950</v>
+      </c>
+      <c r="J13" s="22" t="n">
+        <v>78</v>
+      </c>
+      <c r="K13" s="22" t="n">
+        <v>212</v>
+      </c>
+      <c r="L13" s="24" t="n">
+        <v>245</v>
+      </c>
+      <c r="M13" s="24" t="n">
+        <v>559</v>
+      </c>
+      <c r="N13" s="24" t="n">
+        <v>656</v>
+      </c>
+      <c r="O13" s="24" t="n">
+        <v>950</v>
+      </c>
+      <c r="P13" s="24" t="n">
+        <v>1041</v>
+      </c>
+      <c r="Q13" s="24" t="n">
+        <v>1149</v>
+      </c>
+      <c r="R13" s="24" t="n">
+        <v>1182</v>
+      </c>
       <c r="S13" s="22" t="n"/>
       <c r="T13" s="22" t="n"/>
       <c r="U13" s="24" t="n"/>
       <c r="V13" s="24" t="n">
-        <v>-16.33</v>
+        <v>-16.09</v>
       </c>
       <c r="W13" s="24" t="n">
-        <v>40.64</v>
+        <v>41.81</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14" s="14" spans="1:26">
@@ -1359,23 +1395,41 @@
         <v>358</v>
       </c>
       <c r="G15" s="20" t="n">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="H15" s="20" t="n">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="I15" s="20" t="n">
-        <v>1058</v>
-      </c>
-      <c r="J15" s="22" t="n"/>
-      <c r="K15" s="22" t="n"/>
-      <c r="L15" s="24" t="n"/>
-      <c r="M15" s="24" t="n"/>
-      <c r="N15" s="24" t="n"/>
-      <c r="O15" s="24" t="n"/>
-      <c r="P15" s="24" t="n"/>
-      <c r="Q15" s="24" t="n"/>
-      <c r="R15" s="24" t="n"/>
+        <v>996</v>
+      </c>
+      <c r="J15" s="22" t="n">
+        <v>83</v>
+      </c>
+      <c r="K15" s="22" t="n">
+        <v>223</v>
+      </c>
+      <c r="L15" s="24" t="n">
+        <v>242</v>
+      </c>
+      <c r="M15" s="24" t="n">
+        <v>555</v>
+      </c>
+      <c r="N15" s="24" t="n">
+        <v>675</v>
+      </c>
+      <c r="O15" s="24" t="n">
+        <v>996</v>
+      </c>
+      <c r="P15" s="24" t="n">
+        <v>1134</v>
+      </c>
+      <c r="Q15" s="24" t="n">
+        <v>1244</v>
+      </c>
+      <c r="R15" s="24" t="n">
+        <v>1263</v>
+      </c>
       <c r="S15" s="22" t="n"/>
       <c r="T15" s="22" t="n"/>
       <c r="U15" s="24" t="n"/>
@@ -1383,7 +1437,7 @@
         <v>-24.87</v>
       </c>
       <c r="W15" s="24" t="n">
-        <v>40.78</v>
+        <v>41.96</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="16" s="14" spans="1:26">
@@ -1404,31 +1458,49 @@
         <v>399</v>
       </c>
       <c r="G16" s="20" t="n">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="H16" s="20" t="n">
-        <v>1232</v>
+        <v>1189</v>
       </c>
       <c r="I16" s="20" t="n">
-        <v>1084</v>
-      </c>
-      <c r="J16" s="22" t="n"/>
-      <c r="K16" s="22" t="n"/>
-      <c r="L16" s="24" t="n"/>
-      <c r="M16" s="24" t="n"/>
-      <c r="N16" s="24" t="n"/>
-      <c r="O16" s="24" t="n"/>
-      <c r="P16" s="24" t="n"/>
-      <c r="Q16" s="24" t="n"/>
-      <c r="R16" s="24" t="n"/>
+        <v>1065</v>
+      </c>
+      <c r="J16" s="22" t="n">
+        <v>118</v>
+      </c>
+      <c r="K16" s="22" t="n">
+        <v>223</v>
+      </c>
+      <c r="L16" s="24" t="n">
+        <v>306</v>
+      </c>
+      <c r="M16" s="24" t="n">
+        <v>612</v>
+      </c>
+      <c r="N16" s="24" t="n">
+        <v>696</v>
+      </c>
+      <c r="O16" s="24" t="n">
+        <v>1065</v>
+      </c>
+      <c r="P16" s="24" t="n">
+        <v>1189</v>
+      </c>
+      <c r="Q16" s="24" t="n">
+        <v>1290</v>
+      </c>
+      <c r="R16" s="24" t="n">
+        <v>1373</v>
+      </c>
       <c r="S16" s="22" t="n"/>
       <c r="T16" s="22" t="n"/>
       <c r="U16" s="24" t="n"/>
       <c r="V16" s="24" t="n">
-        <v>-7.94</v>
+        <v>-7.24</v>
       </c>
       <c r="W16" s="24" t="n">
-        <v>100.27</v>
+        <v>103.17</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="17" s="14" spans="1:26">
@@ -1613,31 +1685,49 @@
         <v>385</v>
       </c>
       <c r="G21" s="24" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H21" s="24" t="n">
         <v>1216</v>
       </c>
       <c r="I21" s="24" t="n">
-        <v>1113</v>
-      </c>
-      <c r="J21" s="22" t="n"/>
-      <c r="K21" s="22" t="n"/>
-      <c r="L21" s="24" t="n"/>
-      <c r="M21" s="24" t="n"/>
-      <c r="N21" s="24" t="n"/>
-      <c r="O21" s="24" t="n"/>
-      <c r="P21" s="24" t="n"/>
-      <c r="Q21" s="24" t="n"/>
-      <c r="R21" s="24" t="n"/>
+        <v>1122</v>
+      </c>
+      <c r="J21" s="22" t="n">
+        <v>113</v>
+      </c>
+      <c r="K21" s="22" t="n">
+        <v>226</v>
+      </c>
+      <c r="L21" s="24" t="n">
+        <v>244</v>
+      </c>
+      <c r="M21" s="24" t="n">
+        <v>598</v>
+      </c>
+      <c r="N21" s="24" t="n">
+        <v>728</v>
+      </c>
+      <c r="O21" s="24" t="n">
+        <v>1122</v>
+      </c>
+      <c r="P21" s="24" t="n">
+        <v>1216</v>
+      </c>
+      <c r="Q21" s="24" t="n">
+        <v>1333</v>
+      </c>
+      <c r="R21" s="24" t="n">
+        <v>1351</v>
+      </c>
       <c r="S21" s="22" t="n"/>
       <c r="T21" s="22" t="n"/>
       <c r="U21" s="24" t="n"/>
       <c r="V21" s="24" t="n">
-        <v>-15.15</v>
+        <v>-14.82</v>
       </c>
       <c r="W21" s="24" t="n">
-        <v>69.8</v>
+        <v>72.09</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="22" s="14" spans="1:26">
@@ -2008,31 +2098,49 @@
         <v>341</v>
       </c>
       <c r="G30" s="24" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H30" s="24" t="n">
-        <v>1074</v>
+        <v>966</v>
       </c>
       <c r="I30" s="24" t="n">
-        <v>871</v>
-      </c>
-      <c r="J30" s="22" t="n"/>
-      <c r="K30" s="22" t="n"/>
-      <c r="L30" s="24" t="n"/>
-      <c r="M30" s="24" t="n"/>
-      <c r="N30" s="24" t="n"/>
-      <c r="O30" s="24" t="n"/>
-      <c r="P30" s="24" t="n"/>
-      <c r="Q30" s="24" t="n"/>
-      <c r="R30" s="24" t="n"/>
+        <v>860</v>
+      </c>
+      <c r="J30" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="K30" s="22" t="n">
+        <v>987</v>
+      </c>
+      <c r="L30" s="24" t="n">
+        <v>51</v>
+      </c>
+      <c r="M30" s="24" t="n">
+        <v>352</v>
+      </c>
+      <c r="N30" s="24" t="n">
+        <v>445</v>
+      </c>
+      <c r="O30" s="24" t="n">
+        <v>860</v>
+      </c>
+      <c r="P30" s="24" t="n">
+        <v>966</v>
+      </c>
+      <c r="Q30" s="24" t="n">
+        <v>2036</v>
+      </c>
+      <c r="R30" s="24" t="n">
+        <v>1100</v>
+      </c>
       <c r="S30" s="22" t="n"/>
       <c r="T30" s="22" t="n"/>
       <c r="U30" s="24" t="n"/>
       <c r="V30" s="24" t="n">
-        <v>-19.96</v>
+        <v>-19.62</v>
       </c>
       <c r="W30" s="24" t="n">
-        <v>101.56</v>
+        <v>104.51</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="31" s="14" spans="1:26">
@@ -2161,61 +2269,61 @@
       </c>
     </row>
     <row customHeight="1" ht="15" r="34" s="14" spans="1:26">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="13" t="n">
+      <c r="C34" s="24" t="n">
         <v>32</v>
       </c>
-      <c r="D34" s="13" t="n">
+      <c r="D34" s="24" t="n">
         <v>458</v>
       </c>
-      <c r="E34" s="13" t="n">
+      <c r="E34" s="24" t="n">
         <v>54</v>
       </c>
-      <c r="F34" s="13" t="n">
+      <c r="F34" s="24" t="n">
         <v>339</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" s="24" t="n">
         <v>94</v>
       </c>
-      <c r="H34" t="n">
-        <v>1153</v>
-      </c>
-      <c r="I34" t="n">
-        <v>1041</v>
-      </c>
-      <c r="J34" t="n">
+      <c r="H34" s="24" t="n">
+        <v>1158</v>
+      </c>
+      <c r="I34" s="24" t="n">
+        <v>1042</v>
+      </c>
+      <c r="J34" s="13" t="n">
         <v>94</v>
       </c>
-      <c r="K34" t="n">
+      <c r="K34" s="13" t="n">
         <v>658</v>
       </c>
-      <c r="L34" t="n">
+      <c r="L34" s="13" t="n">
         <v>254</v>
       </c>
-      <c r="M34" t="n">
+      <c r="M34" s="13" t="n">
         <v>539</v>
       </c>
-      <c r="N34" t="n">
+      <c r="N34" s="13" t="n">
         <v>232</v>
       </c>
-      <c r="O34" t="n">
-        <v>1041</v>
-      </c>
-      <c r="P34" t="n">
-        <v>1153</v>
-      </c>
-      <c r="Q34" t="n">
+      <c r="O34" s="13" t="n">
+        <v>1042</v>
+      </c>
+      <c r="P34" s="13" t="n">
+        <v>1158</v>
+      </c>
+      <c r="Q34" s="13" t="n">
         <v>1699</v>
       </c>
-      <c r="R34" t="n">
+      <c r="R34" s="13" t="n">
         <v>1295</v>
       </c>
-      <c r="V34" t="n">
-        <v>-16.86</v>
-      </c>
-      <c r="W34" t="n">
+      <c r="V34" s="13" t="n">
+        <v>-16.64</v>
+      </c>
+      <c r="W34" s="13" t="n">
         <v>99.58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GLS is close to D-Station's
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -897,40 +897,40 @@
         <v>382</v>
       </c>
       <c r="G4" s="21" t="n">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="H4" s="21" t="n">
-        <v>1244</v>
+        <v>1151</v>
       </c>
       <c r="I4" s="21" t="n">
-        <v>1162</v>
+        <v>1019</v>
       </c>
       <c r="J4" s="23" t="n">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="K4" s="23" t="n">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="L4" s="21" t="n">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="M4" s="21" t="n">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="N4" s="21" t="n">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="O4" s="21" t="n">
-        <v>1162</v>
+        <v>1019</v>
       </c>
       <c r="P4" s="21" t="n">
-        <v>1244</v>
+        <v>1151</v>
       </c>
       <c r="Q4" s="21" t="n">
-        <v>1352</v>
+        <v>1265</v>
       </c>
       <c r="R4" s="21" t="n">
-        <v>1400</v>
+        <v>1313</v>
       </c>
       <c r="S4" s="23" t="n">
         <v>358</v>
@@ -942,10 +942,10 @@
         <v>0.456632653061225</v>
       </c>
       <c r="V4" s="25" t="n">
-        <v>-16.89</v>
+        <v>-16.81</v>
       </c>
       <c r="W4" s="25" t="n">
-        <v>30.64</v>
+        <v>99.58</v>
       </c>
       <c r="X4" s="16" t="n"/>
       <c r="Y4" s="16" t="n"/>
@@ -1782,16 +1782,16 @@
         <v>384</v>
       </c>
       <c r="G18" s="25" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H18" s="25" t="n">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="I18" s="25" t="n">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="J18" s="23" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K18" s="23" t="n">
         <v>1070</v>
@@ -1806,10 +1806,10 @@
         <v>658</v>
       </c>
       <c r="O18" s="25" t="n">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="P18" s="25" t="n">
-        <v>935</v>
+        <v>942</v>
       </c>
       <c r="Q18" s="25" t="n">
         <v>1958</v>
@@ -1908,16 +1908,16 @@
         <v>385</v>
       </c>
       <c r="G20" s="25" t="n">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H20" s="25" t="n">
-        <v>1215</v>
+        <v>1218</v>
       </c>
       <c r="I20" s="25" t="n">
-        <v>1107</v>
+        <v>1102</v>
       </c>
       <c r="J20" s="23" t="n">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K20" s="23" t="n">
         <v>226</v>
@@ -1932,10 +1932,10 @@
         <v>728</v>
       </c>
       <c r="O20" s="25" t="n">
-        <v>1107</v>
+        <v>1102</v>
       </c>
       <c r="P20" s="25" t="n">
-        <v>1215</v>
+        <v>1218</v>
       </c>
       <c r="Q20" s="25" t="n">
         <v>1333</v>
@@ -2160,16 +2160,16 @@
         <v>354</v>
       </c>
       <c r="G24" s="25" t="n">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="H24" s="25" t="n">
-        <v>1154</v>
+        <v>1159</v>
       </c>
       <c r="I24" s="25" t="n">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="J24" s="23" t="n">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="K24" s="23" t="n">
         <v>996</v>
@@ -2184,10 +2184,10 @@
         <v>599</v>
       </c>
       <c r="O24" s="25" t="n">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="P24" s="25" t="n">
-        <v>1154</v>
+        <v>1159</v>
       </c>
       <c r="Q24" s="25" t="n">
         <v>2037</v>
@@ -2861,46 +2861,46 @@
         <v>348</v>
       </c>
       <c r="G36" s="25" t="n">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="H36" s="25" t="n">
-        <v>1129</v>
+        <v>1476</v>
       </c>
       <c r="I36" s="25" t="n">
-        <v>1020</v>
+        <v>1388</v>
       </c>
       <c r="J36" s="25" t="n">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="K36" s="25" t="n">
-        <v>206</v>
+        <v>259</v>
       </c>
       <c r="L36" s="25" t="n">
-        <v>283</v>
+        <v>336</v>
       </c>
       <c r="M36" s="25" t="n">
-        <v>547</v>
+        <v>600</v>
       </c>
       <c r="N36" s="25" t="n">
-        <v>621</v>
+        <v>674</v>
       </c>
       <c r="O36" s="25" t="n">
-        <v>1020</v>
+        <v>1388</v>
       </c>
       <c r="P36" s="25" t="n">
-        <v>1129</v>
+        <v>1476</v>
       </c>
       <c r="Q36" s="25" t="n">
-        <v>1216</v>
+        <v>1561</v>
       </c>
       <c r="R36" s="25" t="n">
-        <v>1293</v>
+        <v>1638</v>
       </c>
       <c r="V36" s="25" t="n">
-        <v>-19.65</v>
+        <v>-23.03</v>
       </c>
       <c r="W36" s="25" t="n">
-        <v>25.63</v>
+        <v>38.71</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="15" r="37" s="25" spans="1:26">
@@ -3392,16 +3392,16 @@
         <v>436</v>
       </c>
       <c r="G45" s="25" t="n">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="H45" s="25" t="n">
-        <v>1086</v>
+        <v>1076</v>
       </c>
       <c r="I45" s="25" t="n">
         <v>983</v>
       </c>
       <c r="J45" s="25" t="n">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="K45" s="25" t="n">
         <v>219</v>
@@ -3419,7 +3419,7 @@
         <v>983</v>
       </c>
       <c r="P45" s="25" t="n">
-        <v>1086</v>
+        <v>1076</v>
       </c>
       <c r="Q45" s="25" t="n">
         <v>1232</v>

</xml_diff>

<commit_message>
GLS and MD seem to be working after the curves were synced base on 4CH
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -897,16 +897,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="21" t="n">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H4" s="21" t="n">
-        <v>1151</v>
+        <v>1164</v>
       </c>
       <c r="I4" s="21" t="n">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="J4" s="23" t="n">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K4" s="23" t="n">
         <v>224</v>
@@ -921,10 +921,10 @@
         <v>653</v>
       </c>
       <c r="O4" s="21" t="n">
-        <v>1019</v>
+        <v>1025</v>
       </c>
       <c r="P4" s="21" t="n">
-        <v>1151</v>
+        <v>1164</v>
       </c>
       <c r="Q4" s="21" t="n">
         <v>1265</v>
@@ -945,7 +945,7 @@
         <v>-16.81</v>
       </c>
       <c r="W4" s="25" t="n">
-        <v>99.58</v>
+        <v>57.66</v>
       </c>
       <c r="X4" s="16" t="n"/>
       <c r="Y4" s="16" t="n"/>

</xml_diff>

<commit_message>
changed is operator to == (dumbass)
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -897,40 +897,40 @@
         <v>382</v>
       </c>
       <c r="G4" s="21" t="n">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="H4" s="21" t="n">
-        <v>1156</v>
+        <v>1144</v>
       </c>
       <c r="I4" s="21" t="n">
-        <v>1040</v>
+        <v>1015</v>
       </c>
       <c r="J4" s="23" t="n">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="K4" s="23" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L4" s="21" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M4" s="21" t="n">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N4" s="21" t="n">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="O4" s="21" t="n">
-        <v>1040</v>
+        <v>1015</v>
       </c>
       <c r="P4" s="21" t="n">
-        <v>1156</v>
+        <v>1144</v>
       </c>
       <c r="Q4" s="21" t="n">
-        <v>1265</v>
+        <v>1246</v>
       </c>
       <c r="R4" s="21" t="n">
-        <v>1313</v>
+        <v>1294</v>
       </c>
       <c r="S4" s="23" t="n">
         <v>358</v>
@@ -942,10 +942,10 @@
         <v>0.456632653061225</v>
       </c>
       <c r="V4" s="25" t="n">
-        <v>-16.81</v>
+        <v>-17.88</v>
       </c>
       <c r="W4" s="25" t="n">
-        <v>57.66</v>
+        <v>32.25</v>
       </c>
       <c r="X4" s="16" t="n"/>
       <c r="Y4" s="16" t="n"/>

</xml_diff>

<commit_message>
All 6 options working
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -726,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="T14" view="normal" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="V50" activeCellId="0" pane="topLeft" sqref="V50:W53"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="N22" view="normal" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
+      <selection activeCell="A54" activeCellId="0" pane="topLeft" sqref="A54:R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -2034,16 +2034,16 @@
         <v>396</v>
       </c>
       <c r="G21" s="25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="25" t="n">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="I21" s="25" t="n">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="J21" s="23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" s="23" t="n">
         <v>1091</v>
@@ -2058,10 +2058,10 @@
         <v>504</v>
       </c>
       <c r="O21" s="25" t="n">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="P21" s="25" t="n">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="Q21" s="25" t="n">
         <v>2041</v>

</xml_diff>

<commit_message>
Fixed SR from StrainDiff
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -3383,16 +3383,16 @@
         <v>312</v>
       </c>
       <c r="G42" s="25" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H42" s="25" t="n">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="I42" s="25" t="n">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="J42" s="25" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K42" s="25" t="n">
         <v>163</v>
@@ -3407,10 +3407,10 @@
         <v>451</v>
       </c>
       <c r="O42" s="25" t="n">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="P42" s="25" t="n">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="Q42" s="25" t="n">
         <v>750</v>

</xml_diff>

<commit_message>
MD improved(Synced RM_Times), GLS must be reviewed
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -910,16 +910,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="21" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H4" s="21" t="n">
-        <v>1142</v>
+        <v>1146</v>
       </c>
       <c r="I4" s="21" t="n">
-        <v>1020</v>
+        <v>1013</v>
       </c>
       <c r="J4" s="23" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K4" s="23" t="n">
         <v>223</v>
@@ -934,10 +934,10 @@
         <v>652</v>
       </c>
       <c r="O4" s="21" t="n">
-        <v>1020</v>
+        <v>1013</v>
       </c>
       <c r="P4" s="21" t="n">
-        <v>1142</v>
+        <v>1146</v>
       </c>
       <c r="Q4" s="21" t="n">
         <v>1246</v>
@@ -987,10 +987,10 @@
         <v>95</v>
       </c>
       <c r="H5" s="21" t="n">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="I5" s="21" t="n">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="J5" s="23" t="n">
         <v>95</v>
@@ -1008,10 +1008,10 @@
         <v>795</v>
       </c>
       <c r="O5" s="25" t="n">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="P5" s="25" t="n">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="Q5" s="25" t="n">
         <v>1183</v>
@@ -1026,7 +1026,7 @@
         <v>-9.5</v>
       </c>
       <c r="W5" s="25" t="n">
-        <v>144.6</v>
+        <v>87.45</v>
       </c>
       <c r="X5" s="21" t="s">
         <v>26</v>
@@ -1119,10 +1119,10 @@
         <v>3</v>
       </c>
       <c r="H7" s="21" t="n">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="I7" s="21" t="n">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="J7" s="23" t="n">
         <v>3</v>
@@ -1140,10 +1140,10 @@
         <v>420</v>
       </c>
       <c r="O7" s="25" t="n">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="P7" s="25" t="n">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="Q7" s="25" t="n">
         <v>1663</v>
@@ -1374,16 +1374,16 @@
         <v>286</v>
       </c>
       <c r="G11" s="21" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H11" s="21" t="n">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="I11" s="21" t="n">
         <v>694</v>
       </c>
       <c r="J11" s="23" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="K11" s="23" t="n">
         <v>808</v>
@@ -1401,7 +1401,7 @@
         <v>694</v>
       </c>
       <c r="P11" s="25" t="n">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="Q11" s="25" t="n">
         <v>1491</v>
@@ -1509,10 +1509,10 @@
         <v>74</v>
       </c>
       <c r="H13" s="21" t="n">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="I13" s="21" t="n">
-        <v>928</v>
+        <v>937</v>
       </c>
       <c r="J13" s="23" t="n">
         <v>74</v>
@@ -1530,10 +1530,10 @@
         <v>656</v>
       </c>
       <c r="O13" s="25" t="n">
-        <v>928</v>
+        <v>937</v>
       </c>
       <c r="P13" s="25" t="n">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="Q13" s="25" t="n">
         <v>1149</v>
@@ -1968,16 +1968,16 @@
         <v>385</v>
       </c>
       <c r="G20" s="25" t="n">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="H20" s="25" t="n">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="I20" s="25" t="n">
-        <v>1090</v>
+        <v>1110</v>
       </c>
       <c r="J20" s="23" t="n">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="K20" s="23" t="n">
         <v>226</v>
@@ -1992,10 +1992,10 @@
         <v>728</v>
       </c>
       <c r="O20" s="25" t="n">
-        <v>1090</v>
+        <v>1110</v>
       </c>
       <c r="P20" s="25" t="n">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="Q20" s="25" t="n">
         <v>1333</v>
@@ -2232,16 +2232,16 @@
         <v>354</v>
       </c>
       <c r="G24" s="25" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H24" s="25" t="n">
-        <v>1168</v>
+        <v>1174</v>
       </c>
       <c r="I24" s="25" t="n">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="J24" s="23" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K24" s="23" t="n">
         <v>996</v>
@@ -2256,10 +2256,10 @@
         <v>599</v>
       </c>
       <c r="O24" s="25" t="n">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="P24" s="25" t="n">
-        <v>1168</v>
+        <v>1174</v>
       </c>
       <c r="Q24" s="25" t="n">
         <v>2037</v>
@@ -2298,16 +2298,16 @@
         <v>409</v>
       </c>
       <c r="G25" s="25" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H25" s="25" t="n">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="I25" s="25" t="n">
-        <v>1159</v>
+        <v>1174</v>
       </c>
       <c r="J25" s="23" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K25" s="23" t="n">
         <v>271</v>
@@ -2322,10 +2322,10 @@
         <v>764</v>
       </c>
       <c r="O25" s="25" t="n">
-        <v>1159</v>
+        <v>1174</v>
       </c>
       <c r="P25" s="25" t="n">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="Q25" s="25" t="n">
         <v>1410</v>
@@ -2496,16 +2496,16 @@
         <v>331</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="H28" s="25" t="n">
-        <v>1022</v>
+        <v>974</v>
       </c>
       <c r="I28" s="25" t="n">
-        <v>942</v>
+        <v>890</v>
       </c>
       <c r="J28" s="23" t="n">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="K28" s="23" t="n">
         <v>1005</v>
@@ -2520,10 +2520,10 @@
         <v>587</v>
       </c>
       <c r="O28" s="25" t="n">
-        <v>942</v>
+        <v>890</v>
       </c>
       <c r="P28" s="25" t="n">
-        <v>1022</v>
+        <v>974</v>
       </c>
       <c r="Q28" s="25" t="n">
         <v>1893</v>
@@ -2562,16 +2562,16 @@
         <v>341</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H29" s="25" t="n">
-        <v>974</v>
+        <v>959</v>
       </c>
       <c r="I29" s="25" t="n">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="J29" s="23" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K29" s="23" t="n">
         <v>987</v>
@@ -2586,10 +2586,10 @@
         <v>445</v>
       </c>
       <c r="O29" s="25" t="n">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="P29" s="25" t="n">
-        <v>974</v>
+        <v>959</v>
       </c>
       <c r="Q29" s="25" t="n">
         <v>2036</v>
@@ -3383,16 +3383,16 @@
         <v>312</v>
       </c>
       <c r="G42" s="25" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H42" s="25" t="n">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="I42" s="25" t="n">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J42" s="25" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K42" s="25" t="n">
         <v>163</v>
@@ -3407,10 +3407,10 @@
         <v>451</v>
       </c>
       <c r="O42" s="25" t="n">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="P42" s="25" t="n">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="Q42" s="25" t="n">
         <v>750</v>
@@ -3422,7 +3422,7 @@
         <v>-5.22</v>
       </c>
       <c r="W42" s="25" t="n">
-        <v>103.59</v>
+        <v>35.29</v>
       </c>
       <c r="X42" s="26" t="s">
         <v>63</v>
@@ -4081,10 +4081,10 @@
         <v>37</v>
       </c>
       <c r="H53" s="25" t="n">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="I53" s="25" t="n">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="J53" s="25" t="n">
         <v>37</v>
@@ -4102,10 +4102,10 @@
         <v>632</v>
       </c>
       <c r="O53" s="25" t="n">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="P53" s="25" t="n">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="Q53" s="25" t="n">
         <v>856</v>
@@ -4120,7 +4120,7 @@
         <v>-9.279999999999999</v>
       </c>
       <c r="W53" s="25" t="n">
-        <v>75.03</v>
+        <v>73.64</v>
       </c>
       <c r="X53" s="25" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
END_Times now get the last item in the sorted list
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -2235,10 +2235,10 @@
         <v>98</v>
       </c>
       <c r="H24" s="25" t="n">
-        <v>1174</v>
+        <v>1158</v>
       </c>
       <c r="I24" s="25" t="n">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="J24" s="23" t="n">
         <v>98</v>
@@ -2256,10 +2256,10 @@
         <v>599</v>
       </c>
       <c r="O24" s="25" t="n">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="P24" s="25" t="n">
-        <v>1174</v>
+        <v>1158</v>
       </c>
       <c r="Q24" s="25" t="n">
         <v>2037</v>
@@ -2271,7 +2271,7 @@
       <c r="T24" s="23" t="n"/>
       <c r="U24" s="25" t="n"/>
       <c r="V24" s="25" t="n">
-        <v>-16.68</v>
+        <v>-16.73</v>
       </c>
       <c r="W24" s="25" t="n">
         <v>57.66</v>

</xml_diff>

<commit_message>
Corrections for the DIC presentation
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -365,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -404,6 +404,13 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -525,39 +532,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,7 +572,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -648,8 +655,8 @@
   </sheetPr>
   <dimension ref="A1:AP58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB6" activeCellId="0" sqref="AB6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2:AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,10 +686,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="22.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="10.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="31" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="12.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="12.1"/>

</xml_diff>

<commit_message>
Managed to organise until the end of PlotClick
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -922,16 +922,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="29" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H4" s="29" t="n">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="I4" s="29" t="n">
-        <v>1024</v>
+        <v>1007</v>
       </c>
       <c r="J4" s="31" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K4" s="31" t="n">
         <v>223</v>
@@ -946,10 +946,10 @@
         <v>652</v>
       </c>
       <c r="O4" s="29" t="n">
-        <v>1024</v>
+        <v>1007</v>
       </c>
       <c r="P4" s="29" t="n">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="Q4" s="29" t="n">
         <v>1246</v>
@@ -4918,10 +4918,10 @@
       <c r="AC53" s="24" t="n">
         <v>-10.57867240534003</v>
       </c>
-      <c r="AD53" t="n">
+      <c r="AD53" s="24" t="n">
         <v>3.611199711739031</v>
       </c>
-      <c r="AE53" t="n">
+      <c r="AE53" s="24" t="n">
         <v>-3.855916894216616</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commented dstationplotlib, changed the SR calculation from strain curves
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -922,16 +922,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="29" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H4" s="29" t="n">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="I4" s="29" t="n">
-        <v>1007</v>
+        <v>1031</v>
       </c>
       <c r="J4" s="31" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="K4" s="31" t="n">
         <v>223</v>
@@ -946,10 +946,10 @@
         <v>652</v>
       </c>
       <c r="O4" s="29" t="n">
-        <v>1007</v>
+        <v>1031</v>
       </c>
       <c r="P4" s="29" t="n">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="Q4" s="29" t="n">
         <v>1246</v>

</xml_diff>

<commit_message>
Commented and moved Parameters_Plot
</commit_message>
<xml_diff>
--- a/Event_Timing.xlsx
+++ b/Event_Timing.xlsx
@@ -922,16 +922,16 @@
         <v>382</v>
       </c>
       <c r="G4" s="29" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H4" s="29" t="n">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="I4" s="29" t="n">
-        <v>1031</v>
+        <v>1022</v>
       </c>
       <c r="J4" s="31" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K4" s="31" t="n">
         <v>223</v>
@@ -946,10 +946,10 @@
         <v>652</v>
       </c>
       <c r="O4" s="29" t="n">
-        <v>1031</v>
+        <v>1022</v>
       </c>
       <c r="P4" s="29" t="n">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="Q4" s="29" t="n">
         <v>1246</v>

</xml_diff>